<commit_message>
Complete grades IT 1A, update 1C and 1D
</commit_message>
<xml_diff>
--- a/DCIT 65 - CS 3A/LEC AND LAB - CS 3A.xlsx
+++ b/DCIT 65 - CS 3A/LEC AND LAB - CS 3A.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650"/>
   </bookViews>
   <sheets>
     <sheet name="REGISTRATION" sheetId="1" r:id="rId1"/>
@@ -428,9 +428,6 @@
   </si>
   <si>
     <t>Curriculum Year:</t>
-  </si>
-  <si>
-    <t>FIRST YEAR</t>
   </si>
   <si>
     <t>Semester/Summer,AY</t>
@@ -968,6 +965,9 @@
   </si>
   <si>
     <t>201501-820</t>
+  </si>
+  <si>
+    <t>THIRD YEAR</t>
   </si>
 </sst>
 </file>
@@ -4859,8 +4859,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:R71"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4914,7 +4914,7 @@
     </row>
     <row r="4" spans="1:18" ht="16.5" customHeight="1">
       <c r="A4" s="120" t="s">
-        <v>114</v>
+        <v>293</v>
       </c>
       <c r="B4" s="120"/>
       <c r="C4" s="120"/>
@@ -4950,7 +4950,7 @@
       </c>
       <c r="B6" s="158"/>
       <c r="C6" s="159" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D6" s="159"/>
       <c r="E6" s="160" t="s">
@@ -4977,7 +4977,7 @@
       </c>
       <c r="B7" s="164"/>
       <c r="C7" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>5</v>
@@ -5006,10 +5006,10 @@
       </c>
       <c r="B8" s="146"/>
       <c r="C8" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E8" s="147" t="s">
         <v>10</v>
@@ -5084,19 +5084,19 @@
         <v>1</v>
       </c>
       <c r="B11" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="D11" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="E11" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>179</v>
-      </c>
       <c r="F11" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G11" s="140"/>
       <c r="H11" s="141"/>
@@ -5117,19 +5117,19 @@
         <v>2</v>
       </c>
       <c r="B12" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="D12" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="E12" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>183</v>
-      </c>
       <c r="F12" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G12" s="125"/>
       <c r="H12" s="125"/>
@@ -5142,7 +5142,7 @@
         <v>24</v>
       </c>
       <c r="P12" s="124" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q12" s="124"/>
       <c r="R12" s="124"/>
@@ -5152,19 +5152,19 @@
         <v>3</v>
       </c>
       <c r="B13" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="D13" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="E13" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="E13" s="15" t="s">
-        <v>187</v>
-      </c>
       <c r="F13" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G13" s="125"/>
       <c r="H13" s="125"/>
@@ -5177,7 +5177,7 @@
         <v>25</v>
       </c>
       <c r="P13" s="124" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q13" s="124"/>
       <c r="R13" s="124"/>
@@ -5187,19 +5187,19 @@
         <v>4</v>
       </c>
       <c r="B14" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="D14" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="E14" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>191</v>
-      </c>
       <c r="F14" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G14" s="125"/>
       <c r="H14" s="125"/>
@@ -5212,7 +5212,7 @@
         <v>26</v>
       </c>
       <c r="P14" s="121" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q14" s="122"/>
       <c r="R14" s="123"/>
@@ -5222,19 +5222,19 @@
         <v>5</v>
       </c>
       <c r="B15" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="D15" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="E15" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>195</v>
-      </c>
       <c r="F15" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G15" s="125"/>
       <c r="H15" s="125"/>
@@ -5247,7 +5247,7 @@
         <v>27</v>
       </c>
       <c r="P15" s="121" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q15" s="122"/>
       <c r="R15" s="123"/>
@@ -5257,19 +5257,19 @@
         <v>6</v>
       </c>
       <c r="B16" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="D16" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="E16" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>199</v>
-      </c>
       <c r="F16" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G16" s="125"/>
       <c r="H16" s="125"/>
@@ -5282,7 +5282,7 @@
         <v>29</v>
       </c>
       <c r="P16" s="132" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q16" s="133"/>
       <c r="R16" s="134"/>
@@ -5292,19 +5292,19 @@
         <v>7</v>
       </c>
       <c r="B17" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="D17" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="E17" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="E17" s="15" t="s">
-        <v>203</v>
-      </c>
       <c r="F17" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G17" s="125"/>
       <c r="H17" s="125"/>
@@ -5317,7 +5317,7 @@
         <v>28</v>
       </c>
       <c r="P17" s="121" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q17" s="122"/>
       <c r="R17" s="123"/>
@@ -5327,19 +5327,19 @@
         <v>8</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C18" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="D18" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>205</v>
-      </c>
       <c r="E18" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G18" s="125"/>
       <c r="H18" s="125"/>
@@ -5354,19 +5354,19 @@
         <v>9</v>
       </c>
       <c r="B19" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="D19" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="E19" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="E19" s="15" t="s">
-        <v>209</v>
-      </c>
       <c r="F19" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G19" s="125"/>
       <c r="H19" s="125"/>
@@ -5381,19 +5381,19 @@
         <v>10</v>
       </c>
       <c r="B20" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="D20" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="E20" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="E20" s="15" t="s">
-        <v>213</v>
-      </c>
       <c r="F20" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G20" s="125"/>
       <c r="H20" s="125"/>
@@ -5408,19 +5408,19 @@
         <v>11</v>
       </c>
       <c r="B21" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="D21" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="E21" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="E21" s="15" t="s">
-        <v>217</v>
-      </c>
       <c r="F21" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G21" s="125"/>
       <c r="H21" s="125"/>
@@ -5430,7 +5430,7 @@
       <c r="L21" s="127"/>
       <c r="M21" s="127"/>
       <c r="P21" s="94" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -5438,16 +5438,16 @@
         <v>12</v>
       </c>
       <c r="B22" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="D22" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="D22" s="15" t="s">
-        <v>220</v>
-      </c>
       <c r="E22" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F22" s="16"/>
       <c r="G22" s="125"/>
@@ -5469,19 +5469,19 @@
         <v>13</v>
       </c>
       <c r="B23" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="D23" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="E23" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="E23" s="15" t="s">
-        <v>224</v>
-      </c>
       <c r="F23" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G23" s="125"/>
       <c r="H23" s="125"/>
@@ -5502,19 +5502,19 @@
         <v>14</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C24" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="D24" s="15" t="s">
-        <v>226</v>
-      </c>
       <c r="E24" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G24" s="125"/>
       <c r="H24" s="125"/>
@@ -5535,19 +5535,19 @@
         <v>15</v>
       </c>
       <c r="B25" s="84" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C25" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="D25" s="15" t="s">
         <v>281</v>
       </c>
-      <c r="D25" s="15" t="s">
-        <v>282</v>
-      </c>
       <c r="E25" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G25" s="125"/>
       <c r="H25" s="125"/>
@@ -5568,19 +5568,19 @@
         <v>16</v>
       </c>
       <c r="B26" s="84" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C26" s="84" t="s">
+        <v>226</v>
+      </c>
+      <c r="D26" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="D26" s="15" t="s">
-        <v>228</v>
-      </c>
       <c r="E26" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G26" s="125"/>
       <c r="H26" s="125"/>
@@ -5601,19 +5601,19 @@
         <v>17</v>
       </c>
       <c r="B27" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="D27" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="D27" s="15" t="s">
-        <v>231</v>
-      </c>
       <c r="E27" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G27" s="125"/>
       <c r="H27" s="125"/>
@@ -5634,19 +5634,19 @@
         <v>18</v>
       </c>
       <c r="B28" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="C28" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="D28" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="D28" s="15" t="s">
-        <v>234</v>
-      </c>
       <c r="E28" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G28" s="125"/>
       <c r="H28" s="125"/>
@@ -5667,19 +5667,19 @@
         <v>19</v>
       </c>
       <c r="B29" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="D29" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="D29" s="15" t="s">
-        <v>237</v>
-      </c>
       <c r="E29" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G29" s="125"/>
       <c r="H29" s="125"/>
@@ -5700,19 +5700,19 @@
         <v>20</v>
       </c>
       <c r="B30" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="C30" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="D30" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="D30" s="15" t="s">
-        <v>240</v>
-      </c>
       <c r="E30" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G30" s="125"/>
       <c r="H30" s="125"/>
@@ -5733,19 +5733,19 @@
         <v>21</v>
       </c>
       <c r="B31" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="C31" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="D31" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="D31" s="15" t="s">
-        <v>243</v>
-      </c>
       <c r="E31" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G31" s="125"/>
       <c r="H31" s="125"/>
@@ -5762,19 +5762,19 @@
         <v>22</v>
       </c>
       <c r="B32" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="D32" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="D32" s="15" t="s">
-        <v>246</v>
-      </c>
       <c r="E32" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G32" s="125"/>
       <c r="H32" s="125"/>
@@ -5795,19 +5795,19 @@
         <v>23</v>
       </c>
       <c r="B33" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="C33" s="15" t="s">
         <v>247</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="D33" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="E33" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="D33" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>249</v>
-      </c>
       <c r="F33" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G33" s="125"/>
       <c r="H33" s="125"/>
@@ -5822,19 +5822,19 @@
         <v>24</v>
       </c>
       <c r="B34" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="C34" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="D34" s="15" t="s">
         <v>251</v>
       </c>
-      <c r="D34" s="15" t="s">
-        <v>252</v>
-      </c>
       <c r="E34" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G34" s="125"/>
       <c r="H34" s="125"/>
@@ -5849,19 +5849,19 @@
         <v>25</v>
       </c>
       <c r="B35" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="C35" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="D35" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="D35" s="15" t="s">
-        <v>255</v>
-      </c>
       <c r="E35" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G35" s="125"/>
       <c r="H35" s="125"/>
@@ -5876,19 +5876,19 @@
         <v>26</v>
       </c>
       <c r="B36" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C36" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="D36" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="D36" s="15" t="s">
-        <v>258</v>
-      </c>
       <c r="E36" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G36" s="125"/>
       <c r="H36" s="125"/>
@@ -5903,19 +5903,19 @@
         <v>27</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C37" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="D37" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="E37" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="E37" s="15" t="s">
-        <v>261</v>
-      </c>
       <c r="F37" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G37" s="125"/>
       <c r="H37" s="125"/>
@@ -5930,19 +5930,19 @@
         <v>28</v>
       </c>
       <c r="B38" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="C38" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="D38" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="D38" s="15" t="s">
-        <v>264</v>
-      </c>
       <c r="E38" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G38" s="125"/>
       <c r="H38" s="125"/>
@@ -5957,19 +5957,19 @@
         <v>29</v>
       </c>
       <c r="B39" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="D39" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="D39" s="15" t="s">
-        <v>267</v>
-      </c>
       <c r="E39" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G39" s="125"/>
       <c r="H39" s="125"/>
@@ -5984,19 +5984,19 @@
         <v>30</v>
       </c>
       <c r="B40" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="C40" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="D40" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="D40" s="15" t="s">
-        <v>270</v>
-      </c>
       <c r="E40" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G40" s="125"/>
       <c r="H40" s="125"/>
@@ -6011,19 +6011,19 @@
         <v>31</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C41" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D41" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="E41" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="E41" s="15" t="s">
-        <v>273</v>
-      </c>
       <c r="F41" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G41" s="125"/>
       <c r="H41" s="125"/>
@@ -6038,19 +6038,19 @@
         <v>32</v>
       </c>
       <c r="B42" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="C42" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="D42" s="15" t="s">
         <v>275</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="E42" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="E42" s="15" t="s">
-        <v>277</v>
-      </c>
       <c r="F42" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G42" s="125"/>
       <c r="H42" s="125"/>
@@ -6065,19 +6065,19 @@
         <v>33</v>
       </c>
       <c r="B43" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="C43" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="D43" s="15" t="s">
         <v>279</v>
       </c>
-      <c r="D43" s="15" t="s">
-        <v>280</v>
-      </c>
       <c r="E43" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G43" s="125"/>
       <c r="H43" s="125"/>
@@ -6564,7 +6564,6 @@
       <c r="M71" s="127"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <sortState ref="B11:E33">
     <sortCondition ref="C11:C33"/>
   </sortState>
@@ -7333,7 +7332,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Input" prompt="Academic Year&#10;(YYYY-YYYY)" sqref="P12:R13"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7342,9 +7341,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:CU70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D26" sqref="D26"/>
+      <selection pane="topRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7688,7 +7687,7 @@
       <c r="H6" s="173"/>
       <c r="I6" s="173"/>
       <c r="J6" s="175" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K6" s="175"/>
       <c r="L6" s="175"/>
@@ -7721,7 +7720,7 @@
       <c r="AM6" s="175"/>
       <c r="AN6" s="175"/>
       <c r="AO6" s="175" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AP6" s="175"/>
       <c r="AQ6" s="175"/>
@@ -7855,7 +7854,7 @@
         <v>0.2</v>
       </c>
       <c r="AO7" s="174" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AP7" s="174"/>
       <c r="AQ7" s="174"/>
@@ -7869,7 +7868,7 @@
         <v>0.1</v>
       </c>
       <c r="AV7" s="174" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AW7" s="174"/>
       <c r="AX7" s="174"/>
@@ -7885,11 +7884,11 @@
       <c r="BC7" s="184"/>
       <c r="BD7" s="185"/>
       <c r="BE7" s="174" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="BF7" s="174"/>
       <c r="BG7" s="174" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="BH7" s="174"/>
       <c r="BI7" s="178">
@@ -7967,12 +7966,12 @@
       <c r="B8" s="198"/>
       <c r="C8" s="198"/>
       <c r="D8" s="205" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E8" s="205"/>
       <c r="F8" s="205"/>
       <c r="G8" s="205" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H8" s="205"/>
       <c r="I8" s="205"/>
@@ -10096,15 +10095,15 @@
         <v>Cantal Kristin A.</v>
       </c>
       <c r="D16" s="102">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="E16" s="86">
         <f t="shared" si="43"/>
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="F16" s="89">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>22.2</v>
       </c>
       <c r="G16" s="101">
         <v>66</v>
@@ -10219,11 +10218,11 @@
       </c>
       <c r="BC16" s="92">
         <f t="shared" si="18"/>
-        <v>73.861111111111114</v>
+        <v>81.061111111111117</v>
       </c>
       <c r="BD16" s="92">
         <f t="shared" si="19"/>
-        <v>73.86</v>
+        <v>81.06</v>
       </c>
       <c r="BE16" s="102">
         <v>72</v>
@@ -10359,7 +10358,7 @@
       </c>
       <c r="CS16" s="98">
         <f t="shared" si="41"/>
-        <v>83.646000000000001</v>
+        <v>86.525999999999996</v>
       </c>
       <c r="CT16" s="98">
         <f>IFERROR(VLOOKUP(CS16,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -17290,26 +17289,26 @@
         <v>Versoza Kenneth H</v>
       </c>
       <c r="D41" s="102">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E41" s="86">
         <f t="shared" si="43"/>
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="F41" s="89">
         <f t="shared" si="0"/>
-        <v>19.8</v>
+        <v>22.8</v>
       </c>
       <c r="G41" s="102">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="H41" s="86">
         <f t="shared" si="2"/>
-        <v>83.75</v>
+        <v>90</v>
       </c>
       <c r="I41" s="89">
         <f t="shared" si="1"/>
-        <v>25.125</v>
+        <v>27</v>
       </c>
       <c r="J41" s="102">
         <v>16</v>
@@ -17413,11 +17412,11 @@
       </c>
       <c r="BC41" s="92">
         <f t="shared" si="18"/>
-        <v>78.702777777777783</v>
+        <v>83.577777777777783</v>
       </c>
       <c r="BD41" s="92">
         <f t="shared" si="19"/>
-        <v>78.7</v>
+        <v>83.58</v>
       </c>
       <c r="BE41" s="102">
         <v>95</v>
@@ -17553,11 +17552,11 @@
       </c>
       <c r="CS41" s="98">
         <f t="shared" si="45"/>
-        <v>89.277999999999992</v>
+        <v>91.22999999999999</v>
       </c>
       <c r="CT41" s="98">
         <f>IFERROR(VLOOKUP(CS41,REGISTRATION!$P$22:$Q$32,2),"")</f>
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="CU41" s="87" t="str">
         <f t="shared" si="42"/>
@@ -24912,7 +24911,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Grading System" prompt="Number of Quizzes" sqref="AN7"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -24921,8 +24920,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:P68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView view="pageBreakPreview" zoomScale="60" workbookViewId="0">
+      <selection sqref="A1:P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25010,7 +25009,7 @@
         <v>100</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E6" s="44" t="s">
         <v>21</v>
@@ -25490,7 +25489,7 @@
       </c>
       <c r="C14" s="57">
         <f>'RAW GRADES'!F16</f>
-        <v>15</v>
+        <v>22.2</v>
       </c>
       <c r="D14" s="83">
         <f>'RAW GRADES'!I16</f>
@@ -25510,11 +25509,11 @@
       </c>
       <c r="H14" s="53">
         <f>'RAW GRADES'!BC16</f>
-        <v>73.861111111111114</v>
+        <v>81.061111111111117</v>
       </c>
       <c r="I14" s="53">
         <f>'RAW GRADES'!BD16</f>
-        <v>73.86</v>
+        <v>81.06</v>
       </c>
       <c r="J14" s="52">
         <f>'RAW GRADES'!BK16</f>
@@ -25534,7 +25533,7 @@
       </c>
       <c r="N14" s="58">
         <f>'RAW GRADES'!CS16</f>
-        <v>83.646000000000001</v>
+        <v>86.525999999999996</v>
       </c>
       <c r="O14" s="56">
         <f>'RAW GRADES'!CT16</f>
@@ -27115,11 +27114,11 @@
       </c>
       <c r="C39" s="57">
         <f>'RAW GRADES'!F41</f>
-        <v>19.8</v>
+        <v>22.8</v>
       </c>
       <c r="D39" s="83">
         <f>'RAW GRADES'!I41</f>
-        <v>25.125</v>
+        <v>27</v>
       </c>
       <c r="E39" s="52">
         <f>'RAW GRADES'!AN41</f>
@@ -27135,11 +27134,11 @@
       </c>
       <c r="H39" s="53">
         <f>'RAW GRADES'!BC41</f>
-        <v>78.702777777777783</v>
+        <v>83.577777777777783</v>
       </c>
       <c r="I39" s="53">
         <f>'RAW GRADES'!BD41</f>
-        <v>78.7</v>
+        <v>83.58</v>
       </c>
       <c r="J39" s="52">
         <f>'RAW GRADES'!BK41</f>
@@ -27159,11 +27158,11 @@
       </c>
       <c r="N39" s="58">
         <f>'RAW GRADES'!CS41</f>
-        <v>89.277999999999992</v>
+        <v>91.22999999999999</v>
       </c>
       <c r="O39" s="56">
         <f>'RAW GRADES'!CT41</f>
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="P39" s="59" t="str">
         <f t="shared" si="0"/>
@@ -29074,6 +29073,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="72" orientation="landscape" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -29082,8 +29082,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView view="pageBreakPreview" zoomScale="60" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29233,7 +29233,7 @@
       </c>
       <c r="C15" s="241" t="str">
         <f>REGISTRATION!A4</f>
-        <v>FIRST YEAR</v>
+        <v>THIRD YEAR</v>
       </c>
       <c r="D15" s="241"/>
       <c r="E15" s="241"/>
@@ -29255,7 +29255,7 @@
     <row r="17" spans="1:6">
       <c r="A17" s="60"/>
       <c r="B17" s="62" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C17" s="241" t="str">
         <f>UPPER(CONCATENATE(REGISTRATION!P13," ","SEMESTER"," ","A.Y."," ",REGISTRATION!P12))</f>
@@ -29284,10 +29284,10 @@
         <v>31</v>
       </c>
       <c r="D19" s="242" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" s="247" t="s">
         <v>116</v>
-      </c>
-      <c r="E19" s="247" t="s">
-        <v>117</v>
       </c>
       <c r="F19" s="242" t="s">
         <v>95</v>
@@ -29304,7 +29304,7 @@
     <row r="21" spans="1:6" ht="16.5" thickBot="1">
       <c r="A21" s="244"/>
       <c r="B21" s="64" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C21" s="244"/>
       <c r="D21" s="244"/>
@@ -30100,7 +30100,7 @@
       </c>
       <c r="D53" s="68">
         <f>'DEPT CHAIR'!O39</f>
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="E53" s="69" t="str">
         <f t="shared" si="0"/>
@@ -30138,7 +30138,7 @@
     </row>
     <row r="55" spans="1:6" ht="19.5" thickBot="1">
       <c r="A55" s="225" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B55" s="226"/>
       <c r="C55" s="226"/>
@@ -30173,13 +30173,13 @@
     <row r="59" spans="1:6" ht="16.5" thickBot="1">
       <c r="A59" s="60"/>
       <c r="B59" s="73" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C59" s="60"/>
       <c r="D59" s="60"/>
       <c r="E59" s="252">
         <f ca="1">NOW()</f>
-        <v>43080.66135451389</v>
+        <v>43081.87773078704</v>
       </c>
       <c r="F59" s="252"/>
     </row>
@@ -30192,14 +30192,14 @@
       <c r="C60" s="73"/>
       <c r="D60" s="73"/>
       <c r="E60" s="253" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F60" s="253"/>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="60"/>
       <c r="B61" s="74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C61" s="74"/>
       <c r="D61" s="74"/>
@@ -30328,7 +30328,7 @@
     </row>
     <row r="77" spans="1:6" ht="15.75">
       <c r="A77" s="254" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B77" s="254"/>
       <c r="C77" s="254"/>
@@ -30347,21 +30347,21 @@
     <row r="79" spans="1:6" ht="16.5" thickBot="1">
       <c r="A79" s="60"/>
       <c r="B79" s="78" t="s">
+        <v>136</v>
+      </c>
+      <c r="C79" s="238" t="s">
         <v>137</v>
-      </c>
-      <c r="C79" s="238" t="s">
-        <v>138</v>
       </c>
       <c r="D79" s="239"/>
       <c r="E79" s="240" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F79" s="239"/>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="60"/>
       <c r="B80" s="80" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C80" s="234">
         <f>COUNTIF($D$22:$D$54,"=1.0")+COUNTIF($D$22:$D$54,"=1.25")+(COUNTIF($D$22:$D$54,"=1.50")+COUNTIF($D$22:$D$54,"=1.75"))</f>
@@ -30377,7 +30377,7 @@
     <row r="81" spans="1:6">
       <c r="A81" s="60"/>
       <c r="B81" s="81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C81" s="228">
         <f>COUNTIF($D$22:$D$54,"=2.0")+COUNTIF($D$22:$D$54,"=2.25")+(COUNTIF($D$22:$D$54,"=2.50")+COUNTIF($D$22:$D$54,"=2.75"))</f>
@@ -30393,7 +30393,7 @@
     <row r="82" spans="1:6">
       <c r="A82" s="60"/>
       <c r="B82" s="81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C82" s="228">
         <f>COUNTIF($D$22:$D$54,"=3.0")</f>
@@ -30409,7 +30409,7 @@
     <row r="83" spans="1:6" ht="15.75" customHeight="1">
       <c r="A83" s="60"/>
       <c r="B83" s="81" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C83" s="228">
         <f>COUNTIF($D$22:$D$54,"=5.0")</f>
@@ -30425,7 +30425,7 @@
     <row r="84" spans="1:6">
       <c r="A84" s="60"/>
       <c r="B84" s="81" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C84" s="232">
         <v>0</v>
@@ -30440,7 +30440,7 @@
     <row r="85" spans="1:6">
       <c r="A85" s="60"/>
       <c r="B85" s="81" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C85" s="232">
         <v>0</v>
@@ -30455,7 +30455,7 @@
     <row r="86" spans="1:6" ht="16.5" thickBot="1">
       <c r="A86" s="60"/>
       <c r="B86" s="82" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C86" s="221">
         <f>SUM(C80:D85)</f>
@@ -30495,12 +30495,12 @@
     <row r="90" spans="1:6" ht="15.75">
       <c r="A90" s="60"/>
       <c r="B90" s="77" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C90" s="60"/>
       <c r="D90" s="60"/>
       <c r="E90" s="77" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F90" s="60"/>
     </row>
@@ -30515,12 +30515,12 @@
     <row r="92" spans="1:6">
       <c r="A92" s="60"/>
       <c r="B92" s="74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C92" s="60"/>
       <c r="D92" s="60"/>
       <c r="E92" s="74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F92" s="60"/>
     </row>
@@ -30546,7 +30546,7 @@
       <c r="C94" s="60"/>
       <c r="D94" s="60"/>
       <c r="E94" s="74" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F94" s="60"/>
     </row>
@@ -30585,7 +30585,7 @@
     <row r="99" spans="1:7" ht="15.75">
       <c r="A99" s="60"/>
       <c r="B99" s="77" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C99" s="60"/>
       <c r="D99" s="60"/>
@@ -30604,7 +30604,7 @@
     <row r="101" spans="1:7">
       <c r="A101" s="60"/>
       <c r="B101" s="74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C101" s="60"/>
       <c r="D101" s="60"/>
@@ -30625,7 +30625,7 @@
     <row r="103" spans="1:7">
       <c r="A103" s="60"/>
       <c r="B103" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C103" s="60"/>
       <c r="D103" s="60"/>
@@ -30683,10 +30683,14 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="58" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="72" max="16383" man="1"/>
+  </rowBreaks>
   <ignoredErrors>
     <ignoredError sqref="B82:B83" numberStoredAsText="1"/>
   </ignoredErrors>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -30707,7 +30711,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="19.5" thickBot="1">
       <c r="A1" s="266" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B1" s="267"/>
       <c r="C1" s="267"/>
@@ -30732,25 +30736,25 @@
       <c r="B2" s="41"/>
       <c r="C2" s="107"/>
       <c r="D2" s="263" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E2" s="264"/>
       <c r="F2" s="264"/>
       <c r="G2" s="265"/>
       <c r="H2" s="263" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I2" s="264"/>
       <c r="J2" s="264"/>
       <c r="K2" s="265"/>
       <c r="L2" s="263" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M2" s="264"/>
       <c r="N2" s="264"/>
       <c r="O2" s="265"/>
       <c r="P2" s="263" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Q2" s="264"/>
       <c r="R2" s="265"/>
@@ -30761,52 +30765,52 @@
         <v>90</v>
       </c>
       <c r="C3" s="107" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D3" s="108" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" s="106" t="s">
         <v>149</v>
       </c>
-      <c r="E3" s="106" t="s">
+      <c r="F3" s="106" t="s">
         <v>150</v>
       </c>
-      <c r="F3" s="106" t="s">
+      <c r="G3" s="109" t="s">
         <v>151</v>
       </c>
-      <c r="G3" s="109" t="s">
-        <v>152</v>
-      </c>
       <c r="H3" s="108" t="s">
+        <v>148</v>
+      </c>
+      <c r="I3" s="106" t="s">
         <v>149</v>
       </c>
-      <c r="I3" s="106" t="s">
+      <c r="J3" s="106" t="s">
         <v>150</v>
       </c>
-      <c r="J3" s="106" t="s">
+      <c r="K3" s="109" t="s">
         <v>151</v>
       </c>
-      <c r="K3" s="109" t="s">
-        <v>152</v>
-      </c>
       <c r="L3" s="108" t="s">
+        <v>148</v>
+      </c>
+      <c r="M3" s="106" t="s">
         <v>149</v>
       </c>
-      <c r="M3" s="106" t="s">
+      <c r="N3" s="106" t="s">
         <v>150</v>
       </c>
-      <c r="N3" s="106" t="s">
+      <c r="O3" s="109" t="s">
         <v>151</v>
       </c>
-      <c r="O3" s="109" t="s">
-        <v>152</v>
-      </c>
       <c r="P3" s="108" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q3" s="106" t="s">
         <v>154</v>
       </c>
-      <c r="Q3" s="106" t="s">
+      <c r="R3" s="109" t="s">
         <v>155</v>
-      </c>
-      <c r="R3" s="109" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -31872,7 +31876,7 @@
     <mergeCell ref="A1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -31895,7 +31899,7 @@
         <v>86.188000000000002</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -31904,7 +31908,7 @@
         <v>72.667999999999992</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -31913,7 +31917,7 @@
         <v>83.164000000000001</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -31922,7 +31926,7 @@
         <v>87.259999999999991</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -31931,7 +31935,7 @@
         <v>85.367999999999995</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -31940,16 +31944,16 @@
         <v>70.414000000000001</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="98">
         <f>'RAW GRADES'!CS16</f>
-        <v>83.646000000000001</v>
+        <v>86.525999999999996</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -31958,7 +31962,7 @@
         <v>80.22</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -31967,7 +31971,7 @@
         <v>71.066000000000003</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -31976,7 +31980,7 @@
         <v>81.668000000000006</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -31985,7 +31989,7 @@
         <v>79.864000000000004</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -31994,7 +31998,7 @@
         <v>76.066000000000003</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -32003,7 +32007,7 @@
         <v>78.426000000000002</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -32012,7 +32016,7 @@
         <v>79.135999999999996</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -32021,7 +32025,7 @@
         <v>11.028</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -32030,7 +32034,7 @@
         <v>92.97399999999999</v>
       </c>
       <c r="B16" s="84" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -32039,7 +32043,7 @@
         <v>95.352000000000004</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -32048,7 +32052,7 @@
         <v>83.277999999999992</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -32057,7 +32061,7 @@
         <v>97.506</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -32066,7 +32070,7 @@
         <v>88.744</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -32075,7 +32079,7 @@
         <v>84.436000000000007</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -32084,7 +32088,7 @@
         <v>75.504000000000005</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -32093,7 +32097,7 @@
         <v>70.486000000000004</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -32102,7 +32106,7 @@
         <v>83.240000000000009</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -32111,7 +32115,7 @@
         <v>78.616</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -32120,7 +32124,7 @@
         <v>93.109999999999985</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -32129,7 +32133,7 @@
         <v>81.52600000000001</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -32138,7 +32142,7 @@
         <v>75.98599999999999</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -32147,7 +32151,7 @@
         <v>89.256</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -32156,7 +32160,7 @@
         <v>85.41</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -32165,16 +32169,16 @@
         <v>73.76400000000001</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="98">
         <f>'RAW GRADES'!CS41</f>
-        <v>89.277999999999992</v>
+        <v>91.22999999999999</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -32183,7 +32187,7 @@
         <v>81.638000000000005</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish grades it1a, cs3a-c
</commit_message>
<xml_diff>
--- a/DCIT 65 - CS 3A/LEC AND LAB - CS 3A.xlsx
+++ b/DCIT 65 - CS 3A/LEC AND LAB - CS 3A.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="REGISTRATION" sheetId="1" r:id="rId1"/>
@@ -2355,99 +2355,37 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2487,137 +2425,104 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2658,6 +2563,101 @@
     </xf>
     <xf numFmtId="9" fontId="32" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2716,6 +2716,102 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -2789,102 +2885,6 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4848,7 +4848,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4859,7 +4859,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:M4"/>
     </sheetView>
   </sheetViews>
@@ -4881,82 +4881,82 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="160" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-      <c r="L2" s="128"/>
-      <c r="M2" s="128"/>
+      <c r="B2" s="160"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="160"/>
+      <c r="F2" s="160"/>
+      <c r="G2" s="160"/>
+      <c r="H2" s="160"/>
+      <c r="I2" s="160"/>
+      <c r="J2" s="160"/>
+      <c r="K2" s="160"/>
+      <c r="L2" s="160"/>
+      <c r="M2" s="160"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="128"/>
-      <c r="B3" s="128"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="128"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="128"/>
-      <c r="L3" s="128"/>
-      <c r="M3" s="128"/>
+      <c r="A3" s="160"/>
+      <c r="B3" s="160"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="160"/>
+      <c r="F3" s="160"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="160"/>
+      <c r="J3" s="160"/>
+      <c r="K3" s="160"/>
+      <c r="L3" s="160"/>
+      <c r="M3" s="160"/>
     </row>
     <row r="4" spans="1:18" ht="16.5" customHeight="1">
-      <c r="A4" s="120" t="s">
+      <c r="A4" s="155" t="s">
         <v>293</v>
       </c>
-      <c r="B4" s="120"/>
-      <c r="C4" s="120"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120"/>
-      <c r="G4" s="120"/>
-      <c r="H4" s="120"/>
-      <c r="I4" s="120"/>
-      <c r="J4" s="120"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="120"/>
-      <c r="M4" s="120"/>
+      <c r="B4" s="155"/>
+      <c r="C4" s="155"/>
+      <c r="D4" s="155"/>
+      <c r="E4" s="155"/>
+      <c r="F4" s="155"/>
+      <c r="G4" s="155"/>
+      <c r="H4" s="155"/>
+      <c r="I4" s="155"/>
+      <c r="J4" s="155"/>
+      <c r="K4" s="155"/>
+      <c r="L4" s="155"/>
+      <c r="M4" s="155"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A5" s="119"/>
-      <c r="B5" s="119"/>
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119"/>
-      <c r="K5" s="119"/>
-      <c r="L5" s="119"/>
-      <c r="M5" s="119"/>
+      <c r="A5" s="154"/>
+      <c r="B5" s="154"/>
+      <c r="C5" s="154"/>
+      <c r="D5" s="154"/>
+      <c r="E5" s="154"/>
+      <c r="F5" s="154"/>
+      <c r="G5" s="154"/>
+      <c r="H5" s="154"/>
+      <c r="I5" s="154"/>
+      <c r="J5" s="154"/>
+      <c r="K5" s="154"/>
+      <c r="L5" s="154"/>
+      <c r="M5" s="154"/>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="157" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="158"/>
-      <c r="C6" s="159" t="s">
+      <c r="A6" s="119" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="120"/>
+      <c r="C6" s="121" t="s">
         <v>159</v>
       </c>
-      <c r="D6" s="159"/>
-      <c r="E6" s="160" t="s">
+      <c r="D6" s="121"/>
+      <c r="E6" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="160"/>
+      <c r="F6" s="122"/>
       <c r="G6" s="1">
         <v>2</v>
       </c>
@@ -4964,28 +4964,28 @@
         <v>2</v>
       </c>
       <c r="I6" s="1"/>
-      <c r="J6" s="161" t="s">
+      <c r="J6" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="161"/>
-      <c r="L6" s="162"/>
-      <c r="M6" s="162"/>
+      <c r="K6" s="123"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="163" t="s">
+      <c r="A7" s="125" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="164"/>
+      <c r="B7" s="126"/>
       <c r="C7" s="3" t="s">
         <v>158</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="165" t="s">
+      <c r="E7" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="165"/>
+      <c r="F7" s="127"/>
       <c r="G7" s="5">
         <v>1</v>
       </c>
@@ -4993,28 +4993,28 @@
         <v>7</v>
       </c>
       <c r="I7" s="7"/>
-      <c r="J7" s="165" t="s">
+      <c r="J7" s="127" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="165"/>
-      <c r="L7" s="166"/>
-      <c r="M7" s="166"/>
+      <c r="K7" s="127"/>
+      <c r="L7" s="128"/>
+      <c r="M7" s="128"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A8" s="145" t="s">
+      <c r="A8" s="129" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="146"/>
+      <c r="B8" s="130"/>
       <c r="C8" s="8" t="s">
         <v>160</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="E8" s="147" t="s">
+      <c r="E8" s="131" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="147"/>
+      <c r="F8" s="131"/>
       <c r="G8" s="10">
         <v>3</v>
       </c>
@@ -5022,45 +5022,45 @@
         <v>11</v>
       </c>
       <c r="I8" s="12"/>
-      <c r="J8" s="147" t="s">
+      <c r="J8" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="147"/>
-      <c r="L8" s="148"/>
-      <c r="M8" s="148"/>
+      <c r="K8" s="131"/>
+      <c r="L8" s="132"/>
+      <c r="M8" s="132"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A9" s="149" t="s">
+      <c r="A9" s="133" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="151" t="s">
+      <c r="B9" s="135" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="153" t="s">
+      <c r="C9" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="153"/>
-      <c r="E9" s="153"/>
-      <c r="F9" s="154" t="s">
+      <c r="D9" s="137"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="154" t="s">
+      <c r="G9" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="156"/>
-      <c r="I9" s="156"/>
-      <c r="J9" s="137" t="s">
+      <c r="H9" s="140"/>
+      <c r="I9" s="140"/>
+      <c r="J9" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="138"/>
-      <c r="L9" s="137" t="s">
+      <c r="K9" s="142"/>
+      <c r="L9" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="138"/>
+      <c r="M9" s="142"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="150"/>
-      <c r="B10" s="152"/>
+      <c r="A10" s="134"/>
+      <c r="B10" s="136"/>
       <c r="C10" s="13" t="s">
         <v>19</v>
       </c>
@@ -5070,14 +5070,14 @@
       <c r="E10" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F10" s="155"/>
-      <c r="G10" s="155"/>
-      <c r="H10" s="155"/>
-      <c r="I10" s="155"/>
-      <c r="J10" s="139"/>
-      <c r="K10" s="139"/>
-      <c r="L10" s="139"/>
-      <c r="M10" s="139"/>
+      <c r="F10" s="139"/>
+      <c r="G10" s="139"/>
+      <c r="H10" s="139"/>
+      <c r="I10" s="139"/>
+      <c r="J10" s="143"/>
+      <c r="K10" s="143"/>
+      <c r="L10" s="143"/>
+      <c r="M10" s="143"/>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="14">
@@ -5098,19 +5098,19 @@
       <c r="F11" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G11" s="140"/>
-      <c r="H11" s="141"/>
-      <c r="I11" s="142"/>
-      <c r="J11" s="143"/>
-      <c r="K11" s="144"/>
-      <c r="L11" s="140"/>
-      <c r="M11" s="142"/>
-      <c r="O11" s="129" t="s">
+      <c r="G11" s="148"/>
+      <c r="H11" s="149"/>
+      <c r="I11" s="150"/>
+      <c r="J11" s="151"/>
+      <c r="K11" s="152"/>
+      <c r="L11" s="148"/>
+      <c r="M11" s="150"/>
+      <c r="O11" s="161" t="s">
         <v>23</v>
       </c>
-      <c r="P11" s="130"/>
-      <c r="Q11" s="130"/>
-      <c r="R11" s="131"/>
+      <c r="P11" s="162"/>
+      <c r="Q11" s="162"/>
+      <c r="R11" s="163"/>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="14">
@@ -5131,21 +5131,21 @@
       <c r="F12" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G12" s="125"/>
-      <c r="H12" s="125"/>
-      <c r="I12" s="125"/>
-      <c r="J12" s="135"/>
-      <c r="K12" s="136"/>
-      <c r="L12" s="127"/>
-      <c r="M12" s="127"/>
+      <c r="G12" s="144"/>
+      <c r="H12" s="144"/>
+      <c r="I12" s="144"/>
+      <c r="J12" s="145"/>
+      <c r="K12" s="146"/>
+      <c r="L12" s="147"/>
+      <c r="M12" s="147"/>
       <c r="O12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="P12" s="124" t="s">
+      <c r="P12" s="159" t="s">
         <v>161</v>
       </c>
-      <c r="Q12" s="124"/>
-      <c r="R12" s="124"/>
+      <c r="Q12" s="159"/>
+      <c r="R12" s="159"/>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="14">
@@ -5166,21 +5166,21 @@
       <c r="F13" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G13" s="125"/>
-      <c r="H13" s="125"/>
-      <c r="I13" s="125"/>
-      <c r="J13" s="135"/>
-      <c r="K13" s="136"/>
-      <c r="L13" s="127"/>
-      <c r="M13" s="127"/>
+      <c r="G13" s="144"/>
+      <c r="H13" s="144"/>
+      <c r="I13" s="144"/>
+      <c r="J13" s="145"/>
+      <c r="K13" s="146"/>
+      <c r="L13" s="147"/>
+      <c r="M13" s="147"/>
       <c r="O13" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="P13" s="124" t="s">
+      <c r="P13" s="159" t="s">
         <v>171</v>
       </c>
-      <c r="Q13" s="124"/>
-      <c r="R13" s="124"/>
+      <c r="Q13" s="159"/>
+      <c r="R13" s="159"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="14">
@@ -5201,21 +5201,21 @@
       <c r="F14" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G14" s="125"/>
-      <c r="H14" s="125"/>
-      <c r="I14" s="125"/>
-      <c r="J14" s="135"/>
-      <c r="K14" s="136"/>
-      <c r="L14" s="127"/>
-      <c r="M14" s="127"/>
+      <c r="G14" s="144"/>
+      <c r="H14" s="144"/>
+      <c r="I14" s="144"/>
+      <c r="J14" s="145"/>
+      <c r="K14" s="146"/>
+      <c r="L14" s="147"/>
+      <c r="M14" s="147"/>
       <c r="O14" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="121" t="s">
+      <c r="P14" s="156" t="s">
         <v>162</v>
       </c>
-      <c r="Q14" s="122"/>
-      <c r="R14" s="123"/>
+      <c r="Q14" s="157"/>
+      <c r="R14" s="158"/>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="14">
@@ -5236,21 +5236,21 @@
       <c r="F15" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G15" s="125"/>
-      <c r="H15" s="125"/>
-      <c r="I15" s="125"/>
-      <c r="J15" s="135"/>
-      <c r="K15" s="136"/>
-      <c r="L15" s="127"/>
-      <c r="M15" s="127"/>
+      <c r="G15" s="144"/>
+      <c r="H15" s="144"/>
+      <c r="I15" s="144"/>
+      <c r="J15" s="145"/>
+      <c r="K15" s="146"/>
+      <c r="L15" s="147"/>
+      <c r="M15" s="147"/>
       <c r="O15" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="P15" s="121" t="s">
+      <c r="P15" s="156" t="s">
         <v>163</v>
       </c>
-      <c r="Q15" s="122"/>
-      <c r="R15" s="123"/>
+      <c r="Q15" s="157"/>
+      <c r="R15" s="158"/>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="14">
@@ -5271,21 +5271,21 @@
       <c r="F16" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G16" s="125"/>
-      <c r="H16" s="125"/>
-      <c r="I16" s="125"/>
-      <c r="J16" s="135"/>
-      <c r="K16" s="136"/>
-      <c r="L16" s="127"/>
-      <c r="M16" s="127"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="145"/>
+      <c r="K16" s="146"/>
+      <c r="L16" s="147"/>
+      <c r="M16" s="147"/>
       <c r="O16" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="P16" s="132" t="s">
+      <c r="P16" s="164" t="s">
         <v>166</v>
       </c>
-      <c r="Q16" s="133"/>
-      <c r="R16" s="134"/>
+      <c r="Q16" s="165"/>
+      <c r="R16" s="166"/>
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="14">
@@ -5306,21 +5306,21 @@
       <c r="F17" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G17" s="125"/>
-      <c r="H17" s="125"/>
-      <c r="I17" s="125"/>
-      <c r="J17" s="135"/>
-      <c r="K17" s="136"/>
-      <c r="L17" s="127"/>
-      <c r="M17" s="127"/>
+      <c r="G17" s="144"/>
+      <c r="H17" s="144"/>
+      <c r="I17" s="144"/>
+      <c r="J17" s="145"/>
+      <c r="K17" s="146"/>
+      <c r="L17" s="147"/>
+      <c r="M17" s="147"/>
       <c r="O17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="P17" s="121" t="s">
+      <c r="P17" s="156" t="s">
         <v>164</v>
       </c>
-      <c r="Q17" s="122"/>
-      <c r="R17" s="123"/>
+      <c r="Q17" s="157"/>
+      <c r="R17" s="158"/>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="14">
@@ -5341,13 +5341,13 @@
       <c r="F18" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G18" s="125"/>
-      <c r="H18" s="125"/>
-      <c r="I18" s="125"/>
-      <c r="J18" s="135"/>
-      <c r="K18" s="136"/>
-      <c r="L18" s="127"/>
-      <c r="M18" s="127"/>
+      <c r="G18" s="144"/>
+      <c r="H18" s="144"/>
+      <c r="I18" s="144"/>
+      <c r="J18" s="145"/>
+      <c r="K18" s="146"/>
+      <c r="L18" s="147"/>
+      <c r="M18" s="147"/>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="14">
@@ -5368,13 +5368,13 @@
       <c r="F19" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G19" s="125"/>
-      <c r="H19" s="125"/>
-      <c r="I19" s="125"/>
-      <c r="J19" s="135"/>
-      <c r="K19" s="136"/>
-      <c r="L19" s="127"/>
-      <c r="M19" s="127"/>
+      <c r="G19" s="144"/>
+      <c r="H19" s="144"/>
+      <c r="I19" s="144"/>
+      <c r="J19" s="145"/>
+      <c r="K19" s="146"/>
+      <c r="L19" s="147"/>
+      <c r="M19" s="147"/>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="14">
@@ -5395,13 +5395,13 @@
       <c r="F20" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G20" s="125"/>
-      <c r="H20" s="125"/>
-      <c r="I20" s="125"/>
-      <c r="J20" s="135"/>
-      <c r="K20" s="136"/>
-      <c r="L20" s="127"/>
-      <c r="M20" s="127"/>
+      <c r="G20" s="144"/>
+      <c r="H20" s="144"/>
+      <c r="I20" s="144"/>
+      <c r="J20" s="145"/>
+      <c r="K20" s="146"/>
+      <c r="L20" s="147"/>
+      <c r="M20" s="147"/>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="14">
@@ -5422,13 +5422,13 @@
       <c r="F21" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G21" s="125"/>
-      <c r="H21" s="125"/>
-      <c r="I21" s="125"/>
-      <c r="J21" s="135"/>
-      <c r="K21" s="136"/>
-      <c r="L21" s="127"/>
-      <c r="M21" s="127"/>
+      <c r="G21" s="144"/>
+      <c r="H21" s="144"/>
+      <c r="I21" s="144"/>
+      <c r="J21" s="145"/>
+      <c r="K21" s="146"/>
+      <c r="L21" s="147"/>
+      <c r="M21" s="147"/>
       <c r="P21" s="94" t="s">
         <v>142</v>
       </c>
@@ -5450,13 +5450,13 @@
         <v>168</v>
       </c>
       <c r="F22" s="16"/>
-      <c r="G22" s="125"/>
-      <c r="H22" s="125"/>
-      <c r="I22" s="125"/>
-      <c r="J22" s="135"/>
-      <c r="K22" s="136"/>
-      <c r="L22" s="127"/>
-      <c r="M22" s="127"/>
+      <c r="G22" s="144"/>
+      <c r="H22" s="144"/>
+      <c r="I22" s="144"/>
+      <c r="J22" s="145"/>
+      <c r="K22" s="146"/>
+      <c r="L22" s="147"/>
+      <c r="M22" s="147"/>
       <c r="P22" s="95">
         <v>0</v>
       </c>
@@ -5483,13 +5483,13 @@
       <c r="F23" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G23" s="125"/>
-      <c r="H23" s="125"/>
-      <c r="I23" s="125"/>
-      <c r="J23" s="135"/>
-      <c r="K23" s="136"/>
-      <c r="L23" s="127"/>
-      <c r="M23" s="127"/>
+      <c r="G23" s="144"/>
+      <c r="H23" s="144"/>
+      <c r="I23" s="144"/>
+      <c r="J23" s="145"/>
+      <c r="K23" s="146"/>
+      <c r="L23" s="147"/>
+      <c r="M23" s="147"/>
       <c r="P23" s="96">
         <v>70</v>
       </c>
@@ -5516,13 +5516,13 @@
       <c r="F24" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G24" s="125"/>
-      <c r="H24" s="125"/>
-      <c r="I24" s="125"/>
-      <c r="J24" s="135"/>
-      <c r="K24" s="136"/>
-      <c r="L24" s="127"/>
-      <c r="M24" s="127"/>
+      <c r="G24" s="144"/>
+      <c r="H24" s="144"/>
+      <c r="I24" s="144"/>
+      <c r="J24" s="145"/>
+      <c r="K24" s="146"/>
+      <c r="L24" s="147"/>
+      <c r="M24" s="147"/>
       <c r="P24" s="96">
         <v>73.34</v>
       </c>
@@ -5549,13 +5549,13 @@
       <c r="F25" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G25" s="125"/>
-      <c r="H25" s="125"/>
-      <c r="I25" s="125"/>
-      <c r="J25" s="135"/>
-      <c r="K25" s="136"/>
-      <c r="L25" s="127"/>
-      <c r="M25" s="127"/>
+      <c r="G25" s="144"/>
+      <c r="H25" s="144"/>
+      <c r="I25" s="144"/>
+      <c r="J25" s="145"/>
+      <c r="K25" s="146"/>
+      <c r="L25" s="147"/>
+      <c r="M25" s="147"/>
       <c r="P25" s="96">
         <v>76.680000000000007</v>
       </c>
@@ -5582,13 +5582,13 @@
       <c r="F26" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G26" s="125"/>
-      <c r="H26" s="125"/>
-      <c r="I26" s="125"/>
-      <c r="J26" s="135"/>
-      <c r="K26" s="136"/>
-      <c r="L26" s="127"/>
-      <c r="M26" s="127"/>
+      <c r="G26" s="144"/>
+      <c r="H26" s="144"/>
+      <c r="I26" s="144"/>
+      <c r="J26" s="145"/>
+      <c r="K26" s="146"/>
+      <c r="L26" s="147"/>
+      <c r="M26" s="147"/>
       <c r="P26" s="96">
         <v>80.02</v>
       </c>
@@ -5615,13 +5615,13 @@
       <c r="F27" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G27" s="125"/>
-      <c r="H27" s="125"/>
-      <c r="I27" s="125"/>
-      <c r="J27" s="135"/>
-      <c r="K27" s="136"/>
-      <c r="L27" s="127"/>
-      <c r="M27" s="127"/>
+      <c r="G27" s="144"/>
+      <c r="H27" s="144"/>
+      <c r="I27" s="144"/>
+      <c r="J27" s="145"/>
+      <c r="K27" s="146"/>
+      <c r="L27" s="147"/>
+      <c r="M27" s="147"/>
       <c r="P27" s="96">
         <v>83.36</v>
       </c>
@@ -5648,13 +5648,13 @@
       <c r="F28" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G28" s="125"/>
-      <c r="H28" s="125"/>
-      <c r="I28" s="125"/>
-      <c r="J28" s="135"/>
-      <c r="K28" s="136"/>
-      <c r="L28" s="127"/>
-      <c r="M28" s="127"/>
+      <c r="G28" s="144"/>
+      <c r="H28" s="144"/>
+      <c r="I28" s="144"/>
+      <c r="J28" s="145"/>
+      <c r="K28" s="146"/>
+      <c r="L28" s="147"/>
+      <c r="M28" s="147"/>
       <c r="P28" s="96">
         <v>86.7</v>
       </c>
@@ -5681,13 +5681,13 @@
       <c r="F29" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G29" s="125"/>
-      <c r="H29" s="125"/>
-      <c r="I29" s="125"/>
-      <c r="J29" s="135"/>
-      <c r="K29" s="136"/>
-      <c r="L29" s="127"/>
-      <c r="M29" s="127"/>
+      <c r="G29" s="144"/>
+      <c r="H29" s="144"/>
+      <c r="I29" s="144"/>
+      <c r="J29" s="145"/>
+      <c r="K29" s="146"/>
+      <c r="L29" s="147"/>
+      <c r="M29" s="147"/>
       <c r="P29" s="96">
         <v>90.04</v>
       </c>
@@ -5714,13 +5714,13 @@
       <c r="F30" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G30" s="125"/>
-      <c r="H30" s="125"/>
-      <c r="I30" s="125"/>
-      <c r="J30" s="135"/>
-      <c r="K30" s="136"/>
-      <c r="L30" s="127"/>
-      <c r="M30" s="127"/>
+      <c r="G30" s="144"/>
+      <c r="H30" s="144"/>
+      <c r="I30" s="144"/>
+      <c r="J30" s="145"/>
+      <c r="K30" s="146"/>
+      <c r="L30" s="147"/>
+      <c r="M30" s="147"/>
       <c r="P30" s="96">
         <v>93.38</v>
       </c>
@@ -5747,13 +5747,13 @@
       <c r="F31" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G31" s="125"/>
-      <c r="H31" s="125"/>
-      <c r="I31" s="125"/>
-      <c r="J31" s="135"/>
-      <c r="K31" s="136"/>
-      <c r="L31" s="127"/>
-      <c r="M31" s="127"/>
+      <c r="G31" s="144"/>
+      <c r="H31" s="144"/>
+      <c r="I31" s="144"/>
+      <c r="J31" s="145"/>
+      <c r="K31" s="146"/>
+      <c r="L31" s="147"/>
+      <c r="M31" s="147"/>
       <c r="P31" s="95"/>
       <c r="Q31" s="95"/>
     </row>
@@ -5776,13 +5776,13 @@
       <c r="F32" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G32" s="125"/>
-      <c r="H32" s="125"/>
-      <c r="I32" s="125"/>
-      <c r="J32" s="135"/>
-      <c r="K32" s="136"/>
-      <c r="L32" s="127"/>
-      <c r="M32" s="127"/>
+      <c r="G32" s="144"/>
+      <c r="H32" s="144"/>
+      <c r="I32" s="144"/>
+      <c r="J32" s="145"/>
+      <c r="K32" s="146"/>
+      <c r="L32" s="147"/>
+      <c r="M32" s="147"/>
       <c r="P32" s="95">
         <v>96.72</v>
       </c>
@@ -5809,13 +5809,13 @@
       <c r="F33" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G33" s="125"/>
-      <c r="H33" s="125"/>
-      <c r="I33" s="125"/>
-      <c r="J33" s="135"/>
-      <c r="K33" s="136"/>
-      <c r="L33" s="127"/>
-      <c r="M33" s="127"/>
+      <c r="G33" s="144"/>
+      <c r="H33" s="144"/>
+      <c r="I33" s="144"/>
+      <c r="J33" s="145"/>
+      <c r="K33" s="146"/>
+      <c r="L33" s="147"/>
+      <c r="M33" s="147"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="14">
@@ -5836,13 +5836,13 @@
       <c r="F34" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G34" s="125"/>
-      <c r="H34" s="125"/>
-      <c r="I34" s="125"/>
-      <c r="J34" s="135"/>
-      <c r="K34" s="136"/>
-      <c r="L34" s="127"/>
-      <c r="M34" s="127"/>
+      <c r="G34" s="144"/>
+      <c r="H34" s="144"/>
+      <c r="I34" s="144"/>
+      <c r="J34" s="145"/>
+      <c r="K34" s="146"/>
+      <c r="L34" s="147"/>
+      <c r="M34" s="147"/>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="14">
@@ -5863,13 +5863,13 @@
       <c r="F35" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G35" s="125"/>
-      <c r="H35" s="125"/>
-      <c r="I35" s="125"/>
-      <c r="J35" s="135"/>
-      <c r="K35" s="136"/>
-      <c r="L35" s="127"/>
-      <c r="M35" s="127"/>
+      <c r="G35" s="144"/>
+      <c r="H35" s="144"/>
+      <c r="I35" s="144"/>
+      <c r="J35" s="145"/>
+      <c r="K35" s="146"/>
+      <c r="L35" s="147"/>
+      <c r="M35" s="147"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="14">
@@ -5890,13 +5890,13 @@
       <c r="F36" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G36" s="125"/>
-      <c r="H36" s="125"/>
-      <c r="I36" s="125"/>
-      <c r="J36" s="135"/>
-      <c r="K36" s="136"/>
-      <c r="L36" s="127"/>
-      <c r="M36" s="127"/>
+      <c r="G36" s="144"/>
+      <c r="H36" s="144"/>
+      <c r="I36" s="144"/>
+      <c r="J36" s="145"/>
+      <c r="K36" s="146"/>
+      <c r="L36" s="147"/>
+      <c r="M36" s="147"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="14">
@@ -5917,13 +5917,13 @@
       <c r="F37" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G37" s="125"/>
-      <c r="H37" s="125"/>
-      <c r="I37" s="125"/>
-      <c r="J37" s="126"/>
-      <c r="K37" s="126"/>
-      <c r="L37" s="127"/>
-      <c r="M37" s="127"/>
+      <c r="G37" s="144"/>
+      <c r="H37" s="144"/>
+      <c r="I37" s="144"/>
+      <c r="J37" s="153"/>
+      <c r="K37" s="153"/>
+      <c r="L37" s="147"/>
+      <c r="M37" s="147"/>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="14">
@@ -5944,13 +5944,13 @@
       <c r="F38" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G38" s="125"/>
-      <c r="H38" s="125"/>
-      <c r="I38" s="125"/>
-      <c r="J38" s="126"/>
-      <c r="K38" s="126"/>
-      <c r="L38" s="127"/>
-      <c r="M38" s="127"/>
+      <c r="G38" s="144"/>
+      <c r="H38" s="144"/>
+      <c r="I38" s="144"/>
+      <c r="J38" s="153"/>
+      <c r="K38" s="153"/>
+      <c r="L38" s="147"/>
+      <c r="M38" s="147"/>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="14">
@@ -5971,13 +5971,13 @@
       <c r="F39" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G39" s="125"/>
-      <c r="H39" s="125"/>
-      <c r="I39" s="125"/>
-      <c r="J39" s="126"/>
-      <c r="K39" s="126"/>
-      <c r="L39" s="127"/>
-      <c r="M39" s="127"/>
+      <c r="G39" s="144"/>
+      <c r="H39" s="144"/>
+      <c r="I39" s="144"/>
+      <c r="J39" s="153"/>
+      <c r="K39" s="153"/>
+      <c r="L39" s="147"/>
+      <c r="M39" s="147"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="14">
@@ -5998,13 +5998,13 @@
       <c r="F40" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G40" s="125"/>
-      <c r="H40" s="125"/>
-      <c r="I40" s="125"/>
-      <c r="J40" s="126"/>
-      <c r="K40" s="126"/>
-      <c r="L40" s="127"/>
-      <c r="M40" s="127"/>
+      <c r="G40" s="144"/>
+      <c r="H40" s="144"/>
+      <c r="I40" s="144"/>
+      <c r="J40" s="153"/>
+      <c r="K40" s="153"/>
+      <c r="L40" s="147"/>
+      <c r="M40" s="147"/>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="14">
@@ -6025,13 +6025,13 @@
       <c r="F41" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G41" s="125"/>
-      <c r="H41" s="125"/>
-      <c r="I41" s="125"/>
-      <c r="J41" s="126"/>
-      <c r="K41" s="126"/>
-      <c r="L41" s="127"/>
-      <c r="M41" s="127"/>
+      <c r="G41" s="144"/>
+      <c r="H41" s="144"/>
+      <c r="I41" s="144"/>
+      <c r="J41" s="153"/>
+      <c r="K41" s="153"/>
+      <c r="L41" s="147"/>
+      <c r="M41" s="147"/>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="14">
@@ -6052,13 +6052,13 @@
       <c r="F42" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G42" s="125"/>
-      <c r="H42" s="125"/>
-      <c r="I42" s="125"/>
-      <c r="J42" s="126"/>
-      <c r="K42" s="126"/>
-      <c r="L42" s="127"/>
-      <c r="M42" s="127"/>
+      <c r="G42" s="144"/>
+      <c r="H42" s="144"/>
+      <c r="I42" s="144"/>
+      <c r="J42" s="153"/>
+      <c r="K42" s="153"/>
+      <c r="L42" s="147"/>
+      <c r="M42" s="147"/>
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="14">
@@ -6079,13 +6079,13 @@
       <c r="F43" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G43" s="125"/>
-      <c r="H43" s="125"/>
-      <c r="I43" s="125"/>
-      <c r="J43" s="126"/>
-      <c r="K43" s="126"/>
-      <c r="L43" s="127"/>
-      <c r="M43" s="127"/>
+      <c r="G43" s="144"/>
+      <c r="H43" s="144"/>
+      <c r="I43" s="144"/>
+      <c r="J43" s="153"/>
+      <c r="K43" s="153"/>
+      <c r="L43" s="147"/>
+      <c r="M43" s="147"/>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="14">
@@ -6096,13 +6096,13 @@
       <c r="D44" s="15"/>
       <c r="E44" s="15"/>
       <c r="F44" s="16"/>
-      <c r="G44" s="125"/>
-      <c r="H44" s="125"/>
-      <c r="I44" s="125"/>
-      <c r="J44" s="126"/>
-      <c r="K44" s="126"/>
-      <c r="L44" s="127"/>
-      <c r="M44" s="127"/>
+      <c r="G44" s="144"/>
+      <c r="H44" s="144"/>
+      <c r="I44" s="144"/>
+      <c r="J44" s="153"/>
+      <c r="K44" s="153"/>
+      <c r="L44" s="147"/>
+      <c r="M44" s="147"/>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="14">
@@ -6113,13 +6113,13 @@
       <c r="D45" s="15"/>
       <c r="E45" s="15"/>
       <c r="F45" s="16"/>
-      <c r="G45" s="125"/>
-      <c r="H45" s="125"/>
-      <c r="I45" s="125"/>
-      <c r="J45" s="126"/>
-      <c r="K45" s="126"/>
-      <c r="L45" s="127"/>
-      <c r="M45" s="127"/>
+      <c r="G45" s="144"/>
+      <c r="H45" s="144"/>
+      <c r="I45" s="144"/>
+      <c r="J45" s="153"/>
+      <c r="K45" s="153"/>
+      <c r="L45" s="147"/>
+      <c r="M45" s="147"/>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="14">
@@ -6130,13 +6130,13 @@
       <c r="D46" s="15"/>
       <c r="E46" s="15"/>
       <c r="F46" s="16"/>
-      <c r="G46" s="125"/>
-      <c r="H46" s="125"/>
-      <c r="I46" s="125"/>
-      <c r="J46" s="126"/>
-      <c r="K46" s="126"/>
-      <c r="L46" s="127"/>
-      <c r="M46" s="127"/>
+      <c r="G46" s="144"/>
+      <c r="H46" s="144"/>
+      <c r="I46" s="144"/>
+      <c r="J46" s="153"/>
+      <c r="K46" s="153"/>
+      <c r="L46" s="147"/>
+      <c r="M46" s="147"/>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="14">
@@ -6147,13 +6147,13 @@
       <c r="D47" s="15"/>
       <c r="E47" s="15"/>
       <c r="F47" s="16"/>
-      <c r="G47" s="125"/>
-      <c r="H47" s="125"/>
-      <c r="I47" s="125"/>
-      <c r="J47" s="126"/>
-      <c r="K47" s="126"/>
-      <c r="L47" s="127"/>
-      <c r="M47" s="127"/>
+      <c r="G47" s="144"/>
+      <c r="H47" s="144"/>
+      <c r="I47" s="144"/>
+      <c r="J47" s="153"/>
+      <c r="K47" s="153"/>
+      <c r="L47" s="147"/>
+      <c r="M47" s="147"/>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="14">
@@ -6164,13 +6164,13 @@
       <c r="D48" s="15"/>
       <c r="E48" s="15"/>
       <c r="F48" s="16"/>
-      <c r="G48" s="125"/>
-      <c r="H48" s="125"/>
-      <c r="I48" s="125"/>
-      <c r="J48" s="126"/>
-      <c r="K48" s="126"/>
-      <c r="L48" s="127"/>
-      <c r="M48" s="127"/>
+      <c r="G48" s="144"/>
+      <c r="H48" s="144"/>
+      <c r="I48" s="144"/>
+      <c r="J48" s="153"/>
+      <c r="K48" s="153"/>
+      <c r="L48" s="147"/>
+      <c r="M48" s="147"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="14">
@@ -6181,13 +6181,13 @@
       <c r="D49" s="15"/>
       <c r="E49" s="15"/>
       <c r="F49" s="16"/>
-      <c r="G49" s="125"/>
-      <c r="H49" s="125"/>
-      <c r="I49" s="125"/>
-      <c r="J49" s="126"/>
-      <c r="K49" s="126"/>
-      <c r="L49" s="127"/>
-      <c r="M49" s="127"/>
+      <c r="G49" s="144"/>
+      <c r="H49" s="144"/>
+      <c r="I49" s="144"/>
+      <c r="J49" s="153"/>
+      <c r="K49" s="153"/>
+      <c r="L49" s="147"/>
+      <c r="M49" s="147"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="14">
@@ -6198,13 +6198,13 @@
       <c r="D50" s="15"/>
       <c r="E50" s="15"/>
       <c r="F50" s="16"/>
-      <c r="G50" s="125"/>
-      <c r="H50" s="125"/>
-      <c r="I50" s="125"/>
-      <c r="J50" s="126"/>
-      <c r="K50" s="126"/>
-      <c r="L50" s="127"/>
-      <c r="M50" s="127"/>
+      <c r="G50" s="144"/>
+      <c r="H50" s="144"/>
+      <c r="I50" s="144"/>
+      <c r="J50" s="153"/>
+      <c r="K50" s="153"/>
+      <c r="L50" s="147"/>
+      <c r="M50" s="147"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="14">
@@ -6215,13 +6215,13 @@
       <c r="D51" s="15"/>
       <c r="E51" s="15"/>
       <c r="F51" s="16"/>
-      <c r="G51" s="125"/>
-      <c r="H51" s="125"/>
-      <c r="I51" s="125"/>
-      <c r="J51" s="126"/>
-      <c r="K51" s="126"/>
-      <c r="L51" s="127"/>
-      <c r="M51" s="127"/>
+      <c r="G51" s="144"/>
+      <c r="H51" s="144"/>
+      <c r="I51" s="144"/>
+      <c r="J51" s="153"/>
+      <c r="K51" s="153"/>
+      <c r="L51" s="147"/>
+      <c r="M51" s="147"/>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="14">
@@ -6232,13 +6232,13 @@
       <c r="D52" s="15"/>
       <c r="E52" s="15"/>
       <c r="F52" s="16"/>
-      <c r="G52" s="125"/>
-      <c r="H52" s="125"/>
-      <c r="I52" s="125"/>
-      <c r="J52" s="126"/>
-      <c r="K52" s="126"/>
-      <c r="L52" s="127"/>
-      <c r="M52" s="127"/>
+      <c r="G52" s="144"/>
+      <c r="H52" s="144"/>
+      <c r="I52" s="144"/>
+      <c r="J52" s="153"/>
+      <c r="K52" s="153"/>
+      <c r="L52" s="147"/>
+      <c r="M52" s="147"/>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="14">
@@ -6249,13 +6249,13 @@
       <c r="D53" s="15"/>
       <c r="E53" s="15"/>
       <c r="F53" s="16"/>
-      <c r="G53" s="125"/>
-      <c r="H53" s="125"/>
-      <c r="I53" s="125"/>
-      <c r="J53" s="126"/>
-      <c r="K53" s="126"/>
-      <c r="L53" s="127"/>
-      <c r="M53" s="127"/>
+      <c r="G53" s="144"/>
+      <c r="H53" s="144"/>
+      <c r="I53" s="144"/>
+      <c r="J53" s="153"/>
+      <c r="K53" s="153"/>
+      <c r="L53" s="147"/>
+      <c r="M53" s="147"/>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="14">
@@ -6266,13 +6266,13 @@
       <c r="D54" s="15"/>
       <c r="E54" s="15"/>
       <c r="F54" s="16"/>
-      <c r="G54" s="125"/>
-      <c r="H54" s="125"/>
-      <c r="I54" s="125"/>
-      <c r="J54" s="126"/>
-      <c r="K54" s="126"/>
-      <c r="L54" s="127"/>
-      <c r="M54" s="127"/>
+      <c r="G54" s="144"/>
+      <c r="H54" s="144"/>
+      <c r="I54" s="144"/>
+      <c r="J54" s="153"/>
+      <c r="K54" s="153"/>
+      <c r="L54" s="147"/>
+      <c r="M54" s="147"/>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="14">
@@ -6283,13 +6283,13 @@
       <c r="D55" s="15"/>
       <c r="E55" s="15"/>
       <c r="F55" s="16"/>
-      <c r="G55" s="125"/>
-      <c r="H55" s="125"/>
-      <c r="I55" s="125"/>
-      <c r="J55" s="126"/>
-      <c r="K55" s="126"/>
-      <c r="L55" s="127"/>
-      <c r="M55" s="127"/>
+      <c r="G55" s="144"/>
+      <c r="H55" s="144"/>
+      <c r="I55" s="144"/>
+      <c r="J55" s="153"/>
+      <c r="K55" s="153"/>
+      <c r="L55" s="147"/>
+      <c r="M55" s="147"/>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="14">
@@ -6300,13 +6300,13 @@
       <c r="D56" s="15"/>
       <c r="E56" s="15"/>
       <c r="F56" s="16"/>
-      <c r="G56" s="125"/>
-      <c r="H56" s="125"/>
-      <c r="I56" s="125"/>
-      <c r="J56" s="126"/>
-      <c r="K56" s="126"/>
-      <c r="L56" s="127"/>
-      <c r="M56" s="127"/>
+      <c r="G56" s="144"/>
+      <c r="H56" s="144"/>
+      <c r="I56" s="144"/>
+      <c r="J56" s="153"/>
+      <c r="K56" s="153"/>
+      <c r="L56" s="147"/>
+      <c r="M56" s="147"/>
     </row>
     <row r="57" spans="1:13">
       <c r="A57" s="14">
@@ -6317,13 +6317,13 @@
       <c r="D57" s="84"/>
       <c r="E57" s="84"/>
       <c r="F57" s="16"/>
-      <c r="G57" s="125"/>
-      <c r="H57" s="125"/>
-      <c r="I57" s="125"/>
-      <c r="J57" s="126"/>
-      <c r="K57" s="126"/>
-      <c r="L57" s="127"/>
-      <c r="M57" s="127"/>
+      <c r="G57" s="144"/>
+      <c r="H57" s="144"/>
+      <c r="I57" s="144"/>
+      <c r="J57" s="153"/>
+      <c r="K57" s="153"/>
+      <c r="L57" s="147"/>
+      <c r="M57" s="147"/>
     </row>
     <row r="58" spans="1:13">
       <c r="A58" s="14">
@@ -6334,13 +6334,13 @@
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
       <c r="F58" s="16"/>
-      <c r="G58" s="125"/>
-      <c r="H58" s="125"/>
-      <c r="I58" s="125"/>
-      <c r="J58" s="126"/>
-      <c r="K58" s="126"/>
-      <c r="L58" s="127"/>
-      <c r="M58" s="127"/>
+      <c r="G58" s="144"/>
+      <c r="H58" s="144"/>
+      <c r="I58" s="144"/>
+      <c r="J58" s="153"/>
+      <c r="K58" s="153"/>
+      <c r="L58" s="147"/>
+      <c r="M58" s="147"/>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="14">
@@ -6351,13 +6351,13 @@
       <c r="D59" s="84"/>
       <c r="E59" s="84"/>
       <c r="F59" s="16"/>
-      <c r="G59" s="125"/>
-      <c r="H59" s="125"/>
-      <c r="I59" s="125"/>
-      <c r="J59" s="126"/>
-      <c r="K59" s="126"/>
-      <c r="L59" s="127"/>
-      <c r="M59" s="127"/>
+      <c r="G59" s="144"/>
+      <c r="H59" s="144"/>
+      <c r="I59" s="144"/>
+      <c r="J59" s="153"/>
+      <c r="K59" s="153"/>
+      <c r="L59" s="147"/>
+      <c r="M59" s="147"/>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="14">
@@ -6368,13 +6368,13 @@
       <c r="D60" s="84"/>
       <c r="E60" s="84"/>
       <c r="F60" s="16"/>
-      <c r="G60" s="125"/>
-      <c r="H60" s="125"/>
-      <c r="I60" s="125"/>
-      <c r="J60" s="126"/>
-      <c r="K60" s="126"/>
-      <c r="L60" s="127"/>
-      <c r="M60" s="127"/>
+      <c r="G60" s="144"/>
+      <c r="H60" s="144"/>
+      <c r="I60" s="144"/>
+      <c r="J60" s="153"/>
+      <c r="K60" s="153"/>
+      <c r="L60" s="147"/>
+      <c r="M60" s="147"/>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="14">
@@ -6385,13 +6385,13 @@
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
       <c r="F61" s="16"/>
-      <c r="G61" s="125"/>
-      <c r="H61" s="125"/>
-      <c r="I61" s="125"/>
-      <c r="J61" s="126"/>
-      <c r="K61" s="126"/>
-      <c r="L61" s="127"/>
-      <c r="M61" s="127"/>
+      <c r="G61" s="144"/>
+      <c r="H61" s="144"/>
+      <c r="I61" s="144"/>
+      <c r="J61" s="153"/>
+      <c r="K61" s="153"/>
+      <c r="L61" s="147"/>
+      <c r="M61" s="147"/>
     </row>
     <row r="62" spans="1:13">
       <c r="A62" s="14">
@@ -6402,13 +6402,13 @@
       <c r="D62" s="15"/>
       <c r="E62" s="15"/>
       <c r="F62" s="16"/>
-      <c r="G62" s="125"/>
-      <c r="H62" s="125"/>
-      <c r="I62" s="125"/>
-      <c r="J62" s="126"/>
-      <c r="K62" s="126"/>
-      <c r="L62" s="127"/>
-      <c r="M62" s="127"/>
+      <c r="G62" s="144"/>
+      <c r="H62" s="144"/>
+      <c r="I62" s="144"/>
+      <c r="J62" s="153"/>
+      <c r="K62" s="153"/>
+      <c r="L62" s="147"/>
+      <c r="M62" s="147"/>
     </row>
     <row r="63" spans="1:13">
       <c r="A63" s="14">
@@ -6419,13 +6419,13 @@
       <c r="D63" s="15"/>
       <c r="E63" s="15"/>
       <c r="F63" s="16"/>
-      <c r="G63" s="125"/>
-      <c r="H63" s="125"/>
-      <c r="I63" s="125"/>
-      <c r="J63" s="126"/>
-      <c r="K63" s="126"/>
-      <c r="L63" s="127"/>
-      <c r="M63" s="127"/>
+      <c r="G63" s="144"/>
+      <c r="H63" s="144"/>
+      <c r="I63" s="144"/>
+      <c r="J63" s="153"/>
+      <c r="K63" s="153"/>
+      <c r="L63" s="147"/>
+      <c r="M63" s="147"/>
     </row>
     <row r="64" spans="1:13">
       <c r="A64" s="14">
@@ -6436,13 +6436,13 @@
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
       <c r="F64" s="16"/>
-      <c r="G64" s="125"/>
-      <c r="H64" s="125"/>
-      <c r="I64" s="125"/>
-      <c r="J64" s="126"/>
-      <c r="K64" s="126"/>
-      <c r="L64" s="127"/>
-      <c r="M64" s="127"/>
+      <c r="G64" s="144"/>
+      <c r="H64" s="144"/>
+      <c r="I64" s="144"/>
+      <c r="J64" s="153"/>
+      <c r="K64" s="153"/>
+      <c r="L64" s="147"/>
+      <c r="M64" s="147"/>
     </row>
     <row r="65" spans="1:13">
       <c r="A65" s="14">
@@ -6453,13 +6453,13 @@
       <c r="D65" s="15"/>
       <c r="E65" s="15"/>
       <c r="F65" s="16"/>
-      <c r="G65" s="125"/>
-      <c r="H65" s="125"/>
-      <c r="I65" s="125"/>
-      <c r="J65" s="126"/>
-      <c r="K65" s="126"/>
-      <c r="L65" s="127"/>
-      <c r="M65" s="127"/>
+      <c r="G65" s="144"/>
+      <c r="H65" s="144"/>
+      <c r="I65" s="144"/>
+      <c r="J65" s="153"/>
+      <c r="K65" s="153"/>
+      <c r="L65" s="147"/>
+      <c r="M65" s="147"/>
     </row>
     <row r="66" spans="1:13">
       <c r="A66" s="14">
@@ -6470,13 +6470,13 @@
       <c r="D66" s="15"/>
       <c r="E66" s="15"/>
       <c r="F66" s="16"/>
-      <c r="G66" s="125"/>
-      <c r="H66" s="125"/>
-      <c r="I66" s="125"/>
-      <c r="J66" s="126"/>
-      <c r="K66" s="126"/>
-      <c r="L66" s="127"/>
-      <c r="M66" s="127"/>
+      <c r="G66" s="144"/>
+      <c r="H66" s="144"/>
+      <c r="I66" s="144"/>
+      <c r="J66" s="153"/>
+      <c r="K66" s="153"/>
+      <c r="L66" s="147"/>
+      <c r="M66" s="147"/>
     </row>
     <row r="67" spans="1:13">
       <c r="A67" s="14">
@@ -6487,13 +6487,13 @@
       <c r="D67" s="15"/>
       <c r="E67" s="84"/>
       <c r="F67" s="16"/>
-      <c r="G67" s="125"/>
-      <c r="H67" s="125"/>
-      <c r="I67" s="125"/>
-      <c r="J67" s="126"/>
-      <c r="K67" s="126"/>
-      <c r="L67" s="127"/>
-      <c r="M67" s="127"/>
+      <c r="G67" s="144"/>
+      <c r="H67" s="144"/>
+      <c r="I67" s="144"/>
+      <c r="J67" s="153"/>
+      <c r="K67" s="153"/>
+      <c r="L67" s="147"/>
+      <c r="M67" s="147"/>
     </row>
     <row r="68" spans="1:13">
       <c r="A68" s="14">
@@ -6504,13 +6504,13 @@
       <c r="D68" s="15"/>
       <c r="E68" s="15"/>
       <c r="F68" s="16"/>
-      <c r="G68" s="125"/>
-      <c r="H68" s="125"/>
-      <c r="I68" s="125"/>
-      <c r="J68" s="126"/>
-      <c r="K68" s="126"/>
-      <c r="L68" s="127"/>
-      <c r="M68" s="127"/>
+      <c r="G68" s="144"/>
+      <c r="H68" s="144"/>
+      <c r="I68" s="144"/>
+      <c r="J68" s="153"/>
+      <c r="K68" s="153"/>
+      <c r="L68" s="147"/>
+      <c r="M68" s="147"/>
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="14">
@@ -6521,13 +6521,13 @@
       <c r="D69" s="15"/>
       <c r="E69" s="15"/>
       <c r="F69" s="16"/>
-      <c r="G69" s="125"/>
-      <c r="H69" s="125"/>
-      <c r="I69" s="125"/>
-      <c r="J69" s="126"/>
-      <c r="K69" s="126"/>
-      <c r="L69" s="127"/>
-      <c r="M69" s="127"/>
+      <c r="G69" s="144"/>
+      <c r="H69" s="144"/>
+      <c r="I69" s="144"/>
+      <c r="J69" s="153"/>
+      <c r="K69" s="153"/>
+      <c r="L69" s="147"/>
+      <c r="M69" s="147"/>
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="14">
@@ -6538,13 +6538,13 @@
       <c r="D70" s="15"/>
       <c r="E70" s="15"/>
       <c r="F70" s="16"/>
-      <c r="G70" s="125"/>
-      <c r="H70" s="125"/>
-      <c r="I70" s="125"/>
-      <c r="J70" s="126"/>
-      <c r="K70" s="126"/>
-      <c r="L70" s="127"/>
-      <c r="M70" s="127"/>
+      <c r="G70" s="144"/>
+      <c r="H70" s="144"/>
+      <c r="I70" s="144"/>
+      <c r="J70" s="153"/>
+      <c r="K70" s="153"/>
+      <c r="L70" s="147"/>
+      <c r="M70" s="147"/>
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="14">
@@ -6555,208 +6555,19 @@
       <c r="D71" s="84"/>
       <c r="E71" s="84"/>
       <c r="F71" s="16"/>
-      <c r="G71" s="125"/>
-      <c r="H71" s="125"/>
-      <c r="I71" s="125"/>
-      <c r="J71" s="126"/>
-      <c r="K71" s="126"/>
-      <c r="L71" s="127"/>
-      <c r="M71" s="127"/>
+      <c r="G71" s="144"/>
+      <c r="H71" s="144"/>
+      <c r="I71" s="144"/>
+      <c r="J71" s="153"/>
+      <c r="K71" s="153"/>
+      <c r="L71" s="147"/>
+      <c r="M71" s="147"/>
     </row>
   </sheetData>
   <sortState ref="B11:E33">
     <sortCondition ref="C11:C33"/>
   </sortState>
   <mergeCells count="213">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:I10"/>
-    <mergeCell ref="J9:K10"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="L9:M10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="L49:M49"/>
-    <mergeCell ref="G50:I50"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="L50:M50"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="G53:I53"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="L53:M53"/>
-    <mergeCell ref="G54:I54"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="L54:M54"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="L51:M51"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="L52:M52"/>
-    <mergeCell ref="G57:I57"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="L57:M57"/>
-    <mergeCell ref="G58:I58"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="L58:M58"/>
-    <mergeCell ref="G55:I55"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="L55:M55"/>
-    <mergeCell ref="G56:I56"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="L56:M56"/>
-    <mergeCell ref="G61:I61"/>
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="L61:M61"/>
-    <mergeCell ref="G62:I62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="L62:M62"/>
-    <mergeCell ref="G59:I59"/>
-    <mergeCell ref="J59:K59"/>
-    <mergeCell ref="L59:M59"/>
-    <mergeCell ref="G60:I60"/>
-    <mergeCell ref="J60:K60"/>
-    <mergeCell ref="L60:M60"/>
-    <mergeCell ref="L68:M68"/>
-    <mergeCell ref="G65:I65"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="L65:M65"/>
-    <mergeCell ref="G66:I66"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="L66:M66"/>
-    <mergeCell ref="G63:I63"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="L63:M63"/>
-    <mergeCell ref="G64:I64"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="L64:M64"/>
     <mergeCell ref="A5:M5"/>
     <mergeCell ref="A4:M4"/>
     <mergeCell ref="P15:R15"/>
@@ -6781,6 +6592,195 @@
     <mergeCell ref="L67:M67"/>
     <mergeCell ref="G68:I68"/>
     <mergeCell ref="J68:K68"/>
+    <mergeCell ref="L68:M68"/>
+    <mergeCell ref="G65:I65"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="L65:M65"/>
+    <mergeCell ref="G66:I66"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="L66:M66"/>
+    <mergeCell ref="G63:I63"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="L63:M63"/>
+    <mergeCell ref="G64:I64"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="L64:M64"/>
+    <mergeCell ref="G61:I61"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="L61:M61"/>
+    <mergeCell ref="G62:I62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="L62:M62"/>
+    <mergeCell ref="G59:I59"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="L59:M59"/>
+    <mergeCell ref="G60:I60"/>
+    <mergeCell ref="J60:K60"/>
+    <mergeCell ref="L60:M60"/>
+    <mergeCell ref="G57:I57"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="L57:M57"/>
+    <mergeCell ref="G58:I58"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="L58:M58"/>
+    <mergeCell ref="G55:I55"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="L55:M55"/>
+    <mergeCell ref="G56:I56"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="L56:M56"/>
+    <mergeCell ref="G53:I53"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="L53:M53"/>
+    <mergeCell ref="G54:I54"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="L54:M54"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="L51:M51"/>
+    <mergeCell ref="G52:I52"/>
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="L52:M52"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="L50:M50"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L9:M10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:I10"/>
+    <mergeCell ref="J9:K10"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
   </mergeCells>
   <conditionalFormatting sqref="B27:B71">
     <cfRule type="cellIs" dxfId="154" priority="115" stopIfTrue="1" operator="equal">
@@ -7357,452 +7357,452 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:99" ht="15" customHeight="1">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="160" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-      <c r="L2" s="128"/>
-      <c r="M2" s="128"/>
-      <c r="N2" s="128"/>
-      <c r="O2" s="128"/>
-      <c r="P2" s="128"/>
-      <c r="Q2" s="128"/>
-      <c r="R2" s="128"/>
-      <c r="S2" s="128"/>
-      <c r="T2" s="128"/>
-      <c r="U2" s="128"/>
-      <c r="V2" s="128"/>
-      <c r="W2" s="128"/>
-      <c r="X2" s="128"/>
-      <c r="Y2" s="128"/>
-      <c r="Z2" s="128"/>
-      <c r="AA2" s="128"/>
-      <c r="AB2" s="128"/>
-      <c r="AC2" s="128"/>
-      <c r="AD2" s="128"/>
-      <c r="AE2" s="128"/>
-      <c r="AF2" s="128"/>
-      <c r="AG2" s="128"/>
-      <c r="AH2" s="128"/>
-      <c r="AI2" s="128"/>
-      <c r="AJ2" s="128"/>
-      <c r="AK2" s="128"/>
-      <c r="AL2" s="128"/>
-      <c r="AM2" s="128"/>
-      <c r="AN2" s="128"/>
-      <c r="AO2" s="128"/>
-      <c r="AP2" s="128"/>
-      <c r="AQ2" s="128"/>
-      <c r="AR2" s="128"/>
-      <c r="AS2" s="128"/>
-      <c r="AT2" s="128"/>
-      <c r="AU2" s="128"/>
-      <c r="AV2" s="128"/>
-      <c r="AW2" s="128"/>
-      <c r="AX2" s="128"/>
-      <c r="AY2" s="128"/>
-      <c r="AZ2" s="128"/>
-      <c r="BA2" s="128"/>
-      <c r="BB2" s="128"/>
-      <c r="BC2" s="128"/>
-      <c r="BD2" s="128"/>
-      <c r="BE2" s="128"/>
-      <c r="BF2" s="128"/>
-      <c r="BG2" s="128"/>
-      <c r="BH2" s="128"/>
-      <c r="BI2" s="128"/>
-      <c r="BJ2" s="128"/>
-      <c r="BK2" s="128"/>
-      <c r="BL2" s="128"/>
-      <c r="BM2" s="128"/>
-      <c r="BN2" s="128"/>
-      <c r="BO2" s="128"/>
-      <c r="BP2" s="128"/>
-      <c r="BQ2" s="128"/>
-      <c r="BR2" s="128"/>
-      <c r="BS2" s="128"/>
-      <c r="BT2" s="128"/>
-      <c r="BU2" s="128"/>
-      <c r="BV2" s="128"/>
-      <c r="BW2" s="128"/>
-      <c r="BX2" s="128"/>
-      <c r="BY2" s="128"/>
-      <c r="BZ2" s="128"/>
-      <c r="CA2" s="128"/>
-      <c r="CB2" s="128"/>
-      <c r="CC2" s="128"/>
-      <c r="CD2" s="128"/>
-      <c r="CE2" s="128"/>
-      <c r="CF2" s="128"/>
-      <c r="CG2" s="128"/>
-      <c r="CH2" s="128"/>
-      <c r="CI2" s="128"/>
-      <c r="CJ2" s="128"/>
-      <c r="CK2" s="128"/>
-      <c r="CL2" s="128"/>
-      <c r="CM2" s="128"/>
-      <c r="CN2" s="128"/>
-      <c r="CO2" s="128"/>
-      <c r="CP2" s="128"/>
-      <c r="CQ2" s="128"/>
-      <c r="CR2" s="128"/>
-      <c r="CS2" s="128"/>
-      <c r="CT2" s="128"/>
-      <c r="CU2" s="128"/>
+      <c r="B2" s="160"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="160"/>
+      <c r="F2" s="160"/>
+      <c r="G2" s="160"/>
+      <c r="H2" s="160"/>
+      <c r="I2" s="160"/>
+      <c r="J2" s="160"/>
+      <c r="K2" s="160"/>
+      <c r="L2" s="160"/>
+      <c r="M2" s="160"/>
+      <c r="N2" s="160"/>
+      <c r="O2" s="160"/>
+      <c r="P2" s="160"/>
+      <c r="Q2" s="160"/>
+      <c r="R2" s="160"/>
+      <c r="S2" s="160"/>
+      <c r="T2" s="160"/>
+      <c r="U2" s="160"/>
+      <c r="V2" s="160"/>
+      <c r="W2" s="160"/>
+      <c r="X2" s="160"/>
+      <c r="Y2" s="160"/>
+      <c r="Z2" s="160"/>
+      <c r="AA2" s="160"/>
+      <c r="AB2" s="160"/>
+      <c r="AC2" s="160"/>
+      <c r="AD2" s="160"/>
+      <c r="AE2" s="160"/>
+      <c r="AF2" s="160"/>
+      <c r="AG2" s="160"/>
+      <c r="AH2" s="160"/>
+      <c r="AI2" s="160"/>
+      <c r="AJ2" s="160"/>
+      <c r="AK2" s="160"/>
+      <c r="AL2" s="160"/>
+      <c r="AM2" s="160"/>
+      <c r="AN2" s="160"/>
+      <c r="AO2" s="160"/>
+      <c r="AP2" s="160"/>
+      <c r="AQ2" s="160"/>
+      <c r="AR2" s="160"/>
+      <c r="AS2" s="160"/>
+      <c r="AT2" s="160"/>
+      <c r="AU2" s="160"/>
+      <c r="AV2" s="160"/>
+      <c r="AW2" s="160"/>
+      <c r="AX2" s="160"/>
+      <c r="AY2" s="160"/>
+      <c r="AZ2" s="160"/>
+      <c r="BA2" s="160"/>
+      <c r="BB2" s="160"/>
+      <c r="BC2" s="160"/>
+      <c r="BD2" s="160"/>
+      <c r="BE2" s="160"/>
+      <c r="BF2" s="160"/>
+      <c r="BG2" s="160"/>
+      <c r="BH2" s="160"/>
+      <c r="BI2" s="160"/>
+      <c r="BJ2" s="160"/>
+      <c r="BK2" s="160"/>
+      <c r="BL2" s="160"/>
+      <c r="BM2" s="160"/>
+      <c r="BN2" s="160"/>
+      <c r="BO2" s="160"/>
+      <c r="BP2" s="160"/>
+      <c r="BQ2" s="160"/>
+      <c r="BR2" s="160"/>
+      <c r="BS2" s="160"/>
+      <c r="BT2" s="160"/>
+      <c r="BU2" s="160"/>
+      <c r="BV2" s="160"/>
+      <c r="BW2" s="160"/>
+      <c r="BX2" s="160"/>
+      <c r="BY2" s="160"/>
+      <c r="BZ2" s="160"/>
+      <c r="CA2" s="160"/>
+      <c r="CB2" s="160"/>
+      <c r="CC2" s="160"/>
+      <c r="CD2" s="160"/>
+      <c r="CE2" s="160"/>
+      <c r="CF2" s="160"/>
+      <c r="CG2" s="160"/>
+      <c r="CH2" s="160"/>
+      <c r="CI2" s="160"/>
+      <c r="CJ2" s="160"/>
+      <c r="CK2" s="160"/>
+      <c r="CL2" s="160"/>
+      <c r="CM2" s="160"/>
+      <c r="CN2" s="160"/>
+      <c r="CO2" s="160"/>
+      <c r="CP2" s="160"/>
+      <c r="CQ2" s="160"/>
+      <c r="CR2" s="160"/>
+      <c r="CS2" s="160"/>
+      <c r="CT2" s="160"/>
+      <c r="CU2" s="160"/>
     </row>
     <row r="3" spans="1:99" ht="15" customHeight="1">
-      <c r="A3" s="128"/>
-      <c r="B3" s="128"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="128"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="128"/>
-      <c r="L3" s="128"/>
-      <c r="M3" s="128"/>
-      <c r="N3" s="128"/>
-      <c r="O3" s="128"/>
-      <c r="P3" s="128"/>
-      <c r="Q3" s="128"/>
-      <c r="R3" s="128"/>
-      <c r="S3" s="128"/>
-      <c r="T3" s="128"/>
-      <c r="U3" s="128"/>
-      <c r="V3" s="128"/>
-      <c r="W3" s="128"/>
-      <c r="X3" s="128"/>
-      <c r="Y3" s="128"/>
-      <c r="Z3" s="128"/>
-      <c r="AA3" s="128"/>
-      <c r="AB3" s="128"/>
-      <c r="AC3" s="128"/>
-      <c r="AD3" s="128"/>
-      <c r="AE3" s="128"/>
-      <c r="AF3" s="128"/>
-      <c r="AG3" s="128"/>
-      <c r="AH3" s="128"/>
-      <c r="AI3" s="128"/>
-      <c r="AJ3" s="128"/>
-      <c r="AK3" s="128"/>
-      <c r="AL3" s="128"/>
-      <c r="AM3" s="128"/>
-      <c r="AN3" s="128"/>
-      <c r="AO3" s="128"/>
-      <c r="AP3" s="128"/>
-      <c r="AQ3" s="128"/>
-      <c r="AR3" s="128"/>
-      <c r="AS3" s="128"/>
-      <c r="AT3" s="128"/>
-      <c r="AU3" s="128"/>
-      <c r="AV3" s="128"/>
-      <c r="AW3" s="128"/>
-      <c r="AX3" s="128"/>
-      <c r="AY3" s="128"/>
-      <c r="AZ3" s="128"/>
-      <c r="BA3" s="128"/>
-      <c r="BB3" s="128"/>
-      <c r="BC3" s="128"/>
-      <c r="BD3" s="128"/>
-      <c r="BE3" s="128"/>
-      <c r="BF3" s="128"/>
-      <c r="BG3" s="128"/>
-      <c r="BH3" s="128"/>
-      <c r="BI3" s="128"/>
-      <c r="BJ3" s="128"/>
-      <c r="BK3" s="128"/>
-      <c r="BL3" s="128"/>
-      <c r="BM3" s="128"/>
-      <c r="BN3" s="128"/>
-      <c r="BO3" s="128"/>
-      <c r="BP3" s="128"/>
-      <c r="BQ3" s="128"/>
-      <c r="BR3" s="128"/>
-      <c r="BS3" s="128"/>
-      <c r="BT3" s="128"/>
-      <c r="BU3" s="128"/>
-      <c r="BV3" s="128"/>
-      <c r="BW3" s="128"/>
-      <c r="BX3" s="128"/>
-      <c r="BY3" s="128"/>
-      <c r="BZ3" s="128"/>
-      <c r="CA3" s="128"/>
-      <c r="CB3" s="128"/>
-      <c r="CC3" s="128"/>
-      <c r="CD3" s="128"/>
-      <c r="CE3" s="128"/>
-      <c r="CF3" s="128"/>
-      <c r="CG3" s="128"/>
-      <c r="CH3" s="128"/>
-      <c r="CI3" s="128"/>
-      <c r="CJ3" s="128"/>
-      <c r="CK3" s="128"/>
-      <c r="CL3" s="128"/>
-      <c r="CM3" s="128"/>
-      <c r="CN3" s="128"/>
-      <c r="CO3" s="128"/>
-      <c r="CP3" s="128"/>
-      <c r="CQ3" s="128"/>
-      <c r="CR3" s="128"/>
-      <c r="CS3" s="128"/>
-      <c r="CT3" s="128"/>
-      <c r="CU3" s="128"/>
+      <c r="A3" s="160"/>
+      <c r="B3" s="160"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="160"/>
+      <c r="F3" s="160"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="160"/>
+      <c r="J3" s="160"/>
+      <c r="K3" s="160"/>
+      <c r="L3" s="160"/>
+      <c r="M3" s="160"/>
+      <c r="N3" s="160"/>
+      <c r="O3" s="160"/>
+      <c r="P3" s="160"/>
+      <c r="Q3" s="160"/>
+      <c r="R3" s="160"/>
+      <c r="S3" s="160"/>
+      <c r="T3" s="160"/>
+      <c r="U3" s="160"/>
+      <c r="V3" s="160"/>
+      <c r="W3" s="160"/>
+      <c r="X3" s="160"/>
+      <c r="Y3" s="160"/>
+      <c r="Z3" s="160"/>
+      <c r="AA3" s="160"/>
+      <c r="AB3" s="160"/>
+      <c r="AC3" s="160"/>
+      <c r="AD3" s="160"/>
+      <c r="AE3" s="160"/>
+      <c r="AF3" s="160"/>
+      <c r="AG3" s="160"/>
+      <c r="AH3" s="160"/>
+      <c r="AI3" s="160"/>
+      <c r="AJ3" s="160"/>
+      <c r="AK3" s="160"/>
+      <c r="AL3" s="160"/>
+      <c r="AM3" s="160"/>
+      <c r="AN3" s="160"/>
+      <c r="AO3" s="160"/>
+      <c r="AP3" s="160"/>
+      <c r="AQ3" s="160"/>
+      <c r="AR3" s="160"/>
+      <c r="AS3" s="160"/>
+      <c r="AT3" s="160"/>
+      <c r="AU3" s="160"/>
+      <c r="AV3" s="160"/>
+      <c r="AW3" s="160"/>
+      <c r="AX3" s="160"/>
+      <c r="AY3" s="160"/>
+      <c r="AZ3" s="160"/>
+      <c r="BA3" s="160"/>
+      <c r="BB3" s="160"/>
+      <c r="BC3" s="160"/>
+      <c r="BD3" s="160"/>
+      <c r="BE3" s="160"/>
+      <c r="BF3" s="160"/>
+      <c r="BG3" s="160"/>
+      <c r="BH3" s="160"/>
+      <c r="BI3" s="160"/>
+      <c r="BJ3" s="160"/>
+      <c r="BK3" s="160"/>
+      <c r="BL3" s="160"/>
+      <c r="BM3" s="160"/>
+      <c r="BN3" s="160"/>
+      <c r="BO3" s="160"/>
+      <c r="BP3" s="160"/>
+      <c r="BQ3" s="160"/>
+      <c r="BR3" s="160"/>
+      <c r="BS3" s="160"/>
+      <c r="BT3" s="160"/>
+      <c r="BU3" s="160"/>
+      <c r="BV3" s="160"/>
+      <c r="BW3" s="160"/>
+      <c r="BX3" s="160"/>
+      <c r="BY3" s="160"/>
+      <c r="BZ3" s="160"/>
+      <c r="CA3" s="160"/>
+      <c r="CB3" s="160"/>
+      <c r="CC3" s="160"/>
+      <c r="CD3" s="160"/>
+      <c r="CE3" s="160"/>
+      <c r="CF3" s="160"/>
+      <c r="CG3" s="160"/>
+      <c r="CH3" s="160"/>
+      <c r="CI3" s="160"/>
+      <c r="CJ3" s="160"/>
+      <c r="CK3" s="160"/>
+      <c r="CL3" s="160"/>
+      <c r="CM3" s="160"/>
+      <c r="CN3" s="160"/>
+      <c r="CO3" s="160"/>
+      <c r="CP3" s="160"/>
+      <c r="CQ3" s="160"/>
+      <c r="CR3" s="160"/>
+      <c r="CS3" s="160"/>
+      <c r="CT3" s="160"/>
+      <c r="CU3" s="160"/>
     </row>
     <row r="4" spans="1:99" ht="15.75" thickBot="1"/>
     <row r="5" spans="1:99" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A5" s="195" t="s">
+      <c r="A5" s="168" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="198" t="s">
+      <c r="B5" s="171" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="198" t="s">
+      <c r="C5" s="171" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="199" t="s">
+      <c r="D5" s="172" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="200"/>
-      <c r="F5" s="200"/>
-      <c r="G5" s="200"/>
-      <c r="H5" s="200"/>
-      <c r="I5" s="200"/>
-      <c r="J5" s="200"/>
-      <c r="K5" s="200"/>
-      <c r="L5" s="200"/>
-      <c r="M5" s="200"/>
-      <c r="N5" s="200"/>
-      <c r="O5" s="200"/>
-      <c r="P5" s="200"/>
-      <c r="Q5" s="200"/>
-      <c r="R5" s="200"/>
-      <c r="S5" s="200"/>
-      <c r="T5" s="200"/>
-      <c r="U5" s="200"/>
-      <c r="V5" s="200"/>
-      <c r="W5" s="200"/>
-      <c r="X5" s="200"/>
-      <c r="Y5" s="200"/>
-      <c r="Z5" s="200"/>
-      <c r="AA5" s="200"/>
-      <c r="AB5" s="200"/>
-      <c r="AC5" s="200"/>
-      <c r="AD5" s="200"/>
-      <c r="AE5" s="200"/>
-      <c r="AF5" s="200"/>
-      <c r="AG5" s="200"/>
-      <c r="AH5" s="200"/>
-      <c r="AI5" s="200"/>
-      <c r="AJ5" s="200"/>
-      <c r="AK5" s="200"/>
-      <c r="AL5" s="200"/>
-      <c r="AM5" s="200"/>
-      <c r="AN5" s="200"/>
-      <c r="AO5" s="200"/>
-      <c r="AP5" s="200"/>
-      <c r="AQ5" s="200"/>
-      <c r="AR5" s="200"/>
-      <c r="AS5" s="200"/>
-      <c r="AT5" s="200"/>
-      <c r="AU5" s="200"/>
-      <c r="AV5" s="200"/>
-      <c r="AW5" s="200"/>
-      <c r="AX5" s="200"/>
-      <c r="AY5" s="200"/>
-      <c r="AZ5" s="200"/>
-      <c r="BA5" s="200"/>
-      <c r="BB5" s="200"/>
-      <c r="BC5" s="200"/>
-      <c r="BD5" s="201"/>
-      <c r="BE5" s="202" t="s">
+      <c r="E5" s="173"/>
+      <c r="F5" s="173"/>
+      <c r="G5" s="173"/>
+      <c r="H5" s="173"/>
+      <c r="I5" s="173"/>
+      <c r="J5" s="173"/>
+      <c r="K5" s="173"/>
+      <c r="L5" s="173"/>
+      <c r="M5" s="173"/>
+      <c r="N5" s="173"/>
+      <c r="O5" s="173"/>
+      <c r="P5" s="173"/>
+      <c r="Q5" s="173"/>
+      <c r="R5" s="173"/>
+      <c r="S5" s="173"/>
+      <c r="T5" s="173"/>
+      <c r="U5" s="173"/>
+      <c r="V5" s="173"/>
+      <c r="W5" s="173"/>
+      <c r="X5" s="173"/>
+      <c r="Y5" s="173"/>
+      <c r="Z5" s="173"/>
+      <c r="AA5" s="173"/>
+      <c r="AB5" s="173"/>
+      <c r="AC5" s="173"/>
+      <c r="AD5" s="173"/>
+      <c r="AE5" s="173"/>
+      <c r="AF5" s="173"/>
+      <c r="AG5" s="173"/>
+      <c r="AH5" s="173"/>
+      <c r="AI5" s="173"/>
+      <c r="AJ5" s="173"/>
+      <c r="AK5" s="173"/>
+      <c r="AL5" s="173"/>
+      <c r="AM5" s="173"/>
+      <c r="AN5" s="173"/>
+      <c r="AO5" s="173"/>
+      <c r="AP5" s="173"/>
+      <c r="AQ5" s="173"/>
+      <c r="AR5" s="173"/>
+      <c r="AS5" s="173"/>
+      <c r="AT5" s="173"/>
+      <c r="AU5" s="173"/>
+      <c r="AV5" s="173"/>
+      <c r="AW5" s="173"/>
+      <c r="AX5" s="173"/>
+      <c r="AY5" s="173"/>
+      <c r="AZ5" s="173"/>
+      <c r="BA5" s="173"/>
+      <c r="BB5" s="173"/>
+      <c r="BC5" s="173"/>
+      <c r="BD5" s="174"/>
+      <c r="BE5" s="175" t="s">
         <v>34</v>
       </c>
-      <c r="BF5" s="203"/>
-      <c r="BG5" s="203"/>
-      <c r="BH5" s="203"/>
-      <c r="BI5" s="203"/>
-      <c r="BJ5" s="203"/>
-      <c r="BK5" s="203"/>
-      <c r="BL5" s="203"/>
-      <c r="BM5" s="203"/>
-      <c r="BN5" s="203"/>
-      <c r="BO5" s="203"/>
-      <c r="BP5" s="203"/>
-      <c r="BQ5" s="203"/>
-      <c r="BR5" s="203"/>
-      <c r="BS5" s="203"/>
-      <c r="BT5" s="203"/>
-      <c r="BU5" s="203"/>
-      <c r="BV5" s="203"/>
-      <c r="BW5" s="203"/>
-      <c r="BX5" s="203"/>
-      <c r="BY5" s="203"/>
-      <c r="BZ5" s="203"/>
-      <c r="CA5" s="203"/>
-      <c r="CB5" s="203"/>
-      <c r="CC5" s="203"/>
-      <c r="CD5" s="203"/>
-      <c r="CE5" s="203"/>
-      <c r="CF5" s="203"/>
-      <c r="CG5" s="203"/>
-      <c r="CH5" s="203"/>
-      <c r="CI5" s="203"/>
-      <c r="CJ5" s="203"/>
-      <c r="CK5" s="203"/>
-      <c r="CL5" s="203"/>
-      <c r="CM5" s="203"/>
-      <c r="CN5" s="203"/>
-      <c r="CO5" s="203"/>
-      <c r="CP5" s="203"/>
-      <c r="CQ5" s="203"/>
-      <c r="CR5" s="204"/>
-      <c r="CS5" s="191" t="s">
+      <c r="BF5" s="176"/>
+      <c r="BG5" s="176"/>
+      <c r="BH5" s="176"/>
+      <c r="BI5" s="176"/>
+      <c r="BJ5" s="176"/>
+      <c r="BK5" s="176"/>
+      <c r="BL5" s="176"/>
+      <c r="BM5" s="176"/>
+      <c r="BN5" s="176"/>
+      <c r="BO5" s="176"/>
+      <c r="BP5" s="176"/>
+      <c r="BQ5" s="176"/>
+      <c r="BR5" s="176"/>
+      <c r="BS5" s="176"/>
+      <c r="BT5" s="176"/>
+      <c r="BU5" s="176"/>
+      <c r="BV5" s="176"/>
+      <c r="BW5" s="176"/>
+      <c r="BX5" s="176"/>
+      <c r="BY5" s="176"/>
+      <c r="BZ5" s="176"/>
+      <c r="CA5" s="176"/>
+      <c r="CB5" s="176"/>
+      <c r="CC5" s="176"/>
+      <c r="CD5" s="176"/>
+      <c r="CE5" s="176"/>
+      <c r="CF5" s="176"/>
+      <c r="CG5" s="176"/>
+      <c r="CH5" s="176"/>
+      <c r="CI5" s="176"/>
+      <c r="CJ5" s="176"/>
+      <c r="CK5" s="176"/>
+      <c r="CL5" s="176"/>
+      <c r="CM5" s="176"/>
+      <c r="CN5" s="176"/>
+      <c r="CO5" s="176"/>
+      <c r="CP5" s="176"/>
+      <c r="CQ5" s="176"/>
+      <c r="CR5" s="177"/>
+      <c r="CS5" s="182" t="s">
         <v>35</v>
       </c>
-      <c r="CT5" s="192"/>
-      <c r="CU5" s="193"/>
+      <c r="CT5" s="183"/>
+      <c r="CU5" s="184"/>
     </row>
     <row r="6" spans="1:99" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A6" s="196"/>
-      <c r="B6" s="198"/>
-      <c r="C6" s="198"/>
-      <c r="D6" s="172" t="s">
+      <c r="A6" s="169"/>
+      <c r="B6" s="171"/>
+      <c r="C6" s="171"/>
+      <c r="D6" s="204" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="173"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="173"/>
-      <c r="H6" s="173"/>
-      <c r="I6" s="173"/>
-      <c r="J6" s="175" t="s">
+      <c r="E6" s="205"/>
+      <c r="F6" s="205"/>
+      <c r="G6" s="205"/>
+      <c r="H6" s="205"/>
+      <c r="I6" s="205"/>
+      <c r="J6" s="188" t="s">
         <v>139</v>
       </c>
-      <c r="K6" s="175"/>
-      <c r="L6" s="175"/>
-      <c r="M6" s="175"/>
-      <c r="N6" s="175"/>
-      <c r="O6" s="175"/>
-      <c r="P6" s="175"/>
-      <c r="Q6" s="175"/>
-      <c r="R6" s="175"/>
-      <c r="S6" s="175"/>
-      <c r="T6" s="175"/>
-      <c r="U6" s="175"/>
-      <c r="V6" s="175"/>
-      <c r="W6" s="175"/>
-      <c r="X6" s="175"/>
-      <c r="Y6" s="175"/>
-      <c r="Z6" s="175"/>
-      <c r="AA6" s="175"/>
-      <c r="AB6" s="175"/>
-      <c r="AC6" s="175"/>
-      <c r="AD6" s="175"/>
-      <c r="AE6" s="175"/>
-      <c r="AF6" s="175"/>
-      <c r="AG6" s="175"/>
-      <c r="AH6" s="175"/>
-      <c r="AI6" s="175"/>
-      <c r="AJ6" s="175"/>
-      <c r="AK6" s="175"/>
-      <c r="AL6" s="175"/>
-      <c r="AM6" s="175"/>
-      <c r="AN6" s="175"/>
-      <c r="AO6" s="175" t="s">
+      <c r="K6" s="188"/>
+      <c r="L6" s="188"/>
+      <c r="M6" s="188"/>
+      <c r="N6" s="188"/>
+      <c r="O6" s="188"/>
+      <c r="P6" s="188"/>
+      <c r="Q6" s="188"/>
+      <c r="R6" s="188"/>
+      <c r="S6" s="188"/>
+      <c r="T6" s="188"/>
+      <c r="U6" s="188"/>
+      <c r="V6" s="188"/>
+      <c r="W6" s="188"/>
+      <c r="X6" s="188"/>
+      <c r="Y6" s="188"/>
+      <c r="Z6" s="188"/>
+      <c r="AA6" s="188"/>
+      <c r="AB6" s="188"/>
+      <c r="AC6" s="188"/>
+      <c r="AD6" s="188"/>
+      <c r="AE6" s="188"/>
+      <c r="AF6" s="188"/>
+      <c r="AG6" s="188"/>
+      <c r="AH6" s="188"/>
+      <c r="AI6" s="188"/>
+      <c r="AJ6" s="188"/>
+      <c r="AK6" s="188"/>
+      <c r="AL6" s="188"/>
+      <c r="AM6" s="188"/>
+      <c r="AN6" s="188"/>
+      <c r="AO6" s="188" t="s">
         <v>140</v>
       </c>
-      <c r="AP6" s="175"/>
-      <c r="AQ6" s="175"/>
-      <c r="AR6" s="175"/>
-      <c r="AS6" s="175" t="s">
+      <c r="AP6" s="188"/>
+      <c r="AQ6" s="188"/>
+      <c r="AR6" s="188"/>
+      <c r="AS6" s="188" t="s">
         <v>37</v>
       </c>
-      <c r="AT6" s="175"/>
-      <c r="AU6" s="175"/>
-      <c r="AV6" s="175" t="s">
+      <c r="AT6" s="188"/>
+      <c r="AU6" s="188"/>
+      <c r="AV6" s="188" t="s">
         <v>38</v>
       </c>
-      <c r="AW6" s="175"/>
-      <c r="AX6" s="175"/>
-      <c r="AY6" s="175"/>
-      <c r="AZ6" s="175"/>
-      <c r="BA6" s="175"/>
-      <c r="BB6" s="175"/>
-      <c r="BC6" s="184" t="s">
+      <c r="AW6" s="188"/>
+      <c r="AX6" s="188"/>
+      <c r="AY6" s="188"/>
+      <c r="AZ6" s="188"/>
+      <c r="BA6" s="188"/>
+      <c r="BB6" s="188"/>
+      <c r="BC6" s="192" t="s">
         <v>39</v>
       </c>
-      <c r="BD6" s="185"/>
-      <c r="BE6" s="186" t="s">
+      <c r="BD6" s="193"/>
+      <c r="BE6" s="194" t="s">
         <v>102</v>
       </c>
-      <c r="BF6" s="187"/>
-      <c r="BG6" s="187"/>
-      <c r="BH6" s="187"/>
-      <c r="BI6" s="187"/>
-      <c r="BJ6" s="187"/>
-      <c r="BK6" s="188"/>
-      <c r="BL6" s="189" t="s">
+      <c r="BF6" s="195"/>
+      <c r="BG6" s="195"/>
+      <c r="BH6" s="195"/>
+      <c r="BI6" s="195"/>
+      <c r="BJ6" s="195"/>
+      <c r="BK6" s="196"/>
+      <c r="BL6" s="197" t="s">
         <v>103</v>
       </c>
-      <c r="BM6" s="187"/>
-      <c r="BN6" s="187"/>
-      <c r="BO6" s="187"/>
-      <c r="BP6" s="187"/>
-      <c r="BQ6" s="187"/>
-      <c r="BR6" s="187"/>
-      <c r="BS6" s="187"/>
-      <c r="BT6" s="187"/>
-      <c r="BU6" s="187"/>
-      <c r="BV6" s="187"/>
-      <c r="BW6" s="187"/>
-      <c r="BX6" s="187"/>
-      <c r="BY6" s="187"/>
-      <c r="BZ6" s="187"/>
-      <c r="CA6" s="187"/>
-      <c r="CB6" s="187"/>
-      <c r="CC6" s="187"/>
-      <c r="CD6" s="187"/>
-      <c r="CE6" s="187"/>
-      <c r="CF6" s="187"/>
-      <c r="CG6" s="187"/>
-      <c r="CH6" s="187"/>
-      <c r="CI6" s="187"/>
-      <c r="CJ6" s="187"/>
-      <c r="CK6" s="187"/>
-      <c r="CL6" s="187"/>
-      <c r="CM6" s="187"/>
-      <c r="CN6" s="187"/>
-      <c r="CO6" s="187"/>
-      <c r="CP6" s="187"/>
-      <c r="CQ6" s="194" t="s">
+      <c r="BM6" s="195"/>
+      <c r="BN6" s="195"/>
+      <c r="BO6" s="195"/>
+      <c r="BP6" s="195"/>
+      <c r="BQ6" s="195"/>
+      <c r="BR6" s="195"/>
+      <c r="BS6" s="195"/>
+      <c r="BT6" s="195"/>
+      <c r="BU6" s="195"/>
+      <c r="BV6" s="195"/>
+      <c r="BW6" s="195"/>
+      <c r="BX6" s="195"/>
+      <c r="BY6" s="195"/>
+      <c r="BZ6" s="195"/>
+      <c r="CA6" s="195"/>
+      <c r="CB6" s="195"/>
+      <c r="CC6" s="195"/>
+      <c r="CD6" s="195"/>
+      <c r="CE6" s="195"/>
+      <c r="CF6" s="195"/>
+      <c r="CG6" s="195"/>
+      <c r="CH6" s="195"/>
+      <c r="CI6" s="195"/>
+      <c r="CJ6" s="195"/>
+      <c r="CK6" s="195"/>
+      <c r="CL6" s="195"/>
+      <c r="CM6" s="195"/>
+      <c r="CN6" s="195"/>
+      <c r="CO6" s="195"/>
+      <c r="CP6" s="195"/>
+      <c r="CQ6" s="185" t="s">
         <v>40</v>
       </c>
-      <c r="CR6" s="194"/>
-      <c r="CS6" s="190" t="s">
+      <c r="CR6" s="185"/>
+      <c r="CS6" s="167" t="s">
         <v>41</v>
       </c>
-      <c r="CT6" s="190" t="s">
+      <c r="CT6" s="167" t="s">
         <v>42</v>
       </c>
-      <c r="CU6" s="181" t="s">
+      <c r="CU6" s="189" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:99" ht="15.75" thickBot="1">
-      <c r="A7" s="196"/>
-      <c r="B7" s="198"/>
-      <c r="C7" s="198"/>
+      <c r="A7" s="169"/>
+      <c r="B7" s="171"/>
+      <c r="C7" s="171"/>
       <c r="E7" s="118"/>
       <c r="F7" s="117">
         <v>0.3</v>
@@ -7811,353 +7811,353 @@
       <c r="I7" s="118">
         <v>0.3</v>
       </c>
-      <c r="J7" s="174">
+      <c r="J7" s="180">
         <v>42980</v>
       </c>
-      <c r="K7" s="174"/>
-      <c r="L7" s="174">
+      <c r="K7" s="180"/>
+      <c r="L7" s="180">
         <v>43035</v>
       </c>
-      <c r="M7" s="174"/>
-      <c r="N7" s="174">
+      <c r="M7" s="180"/>
+      <c r="N7" s="180">
         <v>43056</v>
       </c>
-      <c r="O7" s="174"/>
-      <c r="P7" s="174"/>
-      <c r="Q7" s="174"/>
-      <c r="R7" s="174"/>
-      <c r="S7" s="174"/>
-      <c r="T7" s="180">
+      <c r="O7" s="180"/>
+      <c r="P7" s="180"/>
+      <c r="Q7" s="180"/>
+      <c r="R7" s="180"/>
+      <c r="S7" s="180"/>
+      <c r="T7" s="181">
         <f>COUNT(J9,L9,N9,P9,R9,T9)</f>
         <v>3</v>
       </c>
-      <c r="U7" s="180"/>
-      <c r="V7" s="174"/>
-      <c r="W7" s="174"/>
-      <c r="X7" s="174"/>
-      <c r="Y7" s="174"/>
-      <c r="Z7" s="174"/>
-      <c r="AA7" s="174"/>
-      <c r="AB7" s="174"/>
-      <c r="AC7" s="174"/>
-      <c r="AD7" s="174"/>
-      <c r="AE7" s="174"/>
-      <c r="AF7" s="174"/>
-      <c r="AG7" s="174"/>
-      <c r="AH7" s="174"/>
-      <c r="AI7" s="174"/>
-      <c r="AJ7" s="174"/>
-      <c r="AK7" s="174"/>
-      <c r="AL7" s="174"/>
-      <c r="AM7" s="174"/>
+      <c r="U7" s="181"/>
+      <c r="V7" s="180"/>
+      <c r="W7" s="180"/>
+      <c r="X7" s="180"/>
+      <c r="Y7" s="180"/>
+      <c r="Z7" s="180"/>
+      <c r="AA7" s="180"/>
+      <c r="AB7" s="180"/>
+      <c r="AC7" s="180"/>
+      <c r="AD7" s="180"/>
+      <c r="AE7" s="180"/>
+      <c r="AF7" s="180"/>
+      <c r="AG7" s="180"/>
+      <c r="AH7" s="180"/>
+      <c r="AI7" s="180"/>
+      <c r="AJ7" s="180"/>
+      <c r="AK7" s="180"/>
+      <c r="AL7" s="180"/>
+      <c r="AM7" s="180"/>
       <c r="AN7" s="91">
         <v>0.2</v>
       </c>
-      <c r="AO7" s="174" t="s">
+      <c r="AO7" s="180" t="s">
         <v>286</v>
       </c>
-      <c r="AP7" s="174"/>
-      <c r="AQ7" s="174"/>
-      <c r="AR7" s="174"/>
-      <c r="AS7" s="180">
+      <c r="AP7" s="180"/>
+      <c r="AQ7" s="180"/>
+      <c r="AR7" s="180"/>
+      <c r="AS7" s="181">
         <f>COUNT(AO9,AQ9,AS9)</f>
         <v>1</v>
       </c>
-      <c r="AT7" s="180"/>
+      <c r="AT7" s="181"/>
       <c r="AU7" s="21">
         <v>0.1</v>
       </c>
-      <c r="AV7" s="174" t="s">
+      <c r="AV7" s="180" t="s">
         <v>174</v>
       </c>
-      <c r="AW7" s="174"/>
-      <c r="AX7" s="174"/>
-      <c r="AY7" s="174"/>
-      <c r="AZ7" s="180">
+      <c r="AW7" s="180"/>
+      <c r="AX7" s="180"/>
+      <c r="AY7" s="180"/>
+      <c r="AZ7" s="181">
         <f>COUNT(AV9,AX9,AZ9)</f>
         <v>1</v>
       </c>
-      <c r="BA7" s="180"/>
+      <c r="BA7" s="181"/>
       <c r="BB7" s="22">
         <v>0.1</v>
       </c>
-      <c r="BC7" s="184"/>
-      <c r="BD7" s="185"/>
-      <c r="BE7" s="174" t="s">
+      <c r="BC7" s="192"/>
+      <c r="BD7" s="193"/>
+      <c r="BE7" s="180" t="s">
         <v>287</v>
       </c>
-      <c r="BF7" s="174"/>
-      <c r="BG7" s="174" t="s">
+      <c r="BF7" s="180"/>
+      <c r="BG7" s="180" t="s">
         <v>288</v>
       </c>
-      <c r="BH7" s="174"/>
-      <c r="BI7" s="178">
+      <c r="BH7" s="180"/>
+      <c r="BI7" s="198">
         <f>COUNT(BE9,BG9,BI9)</f>
         <v>3</v>
       </c>
-      <c r="BJ7" s="179"/>
+      <c r="BJ7" s="199"/>
       <c r="BK7" s="99">
         <v>0.5</v>
       </c>
-      <c r="BL7" s="174">
+      <c r="BL7" s="180">
         <v>42980</v>
       </c>
-      <c r="BM7" s="174"/>
-      <c r="BN7" s="174">
+      <c r="BM7" s="180"/>
+      <c r="BN7" s="180">
         <v>42987</v>
       </c>
-      <c r="BO7" s="174"/>
-      <c r="BP7" s="174">
+      <c r="BO7" s="180"/>
+      <c r="BP7" s="180">
         <v>42994</v>
       </c>
-      <c r="BQ7" s="174"/>
-      <c r="BR7" s="174">
+      <c r="BQ7" s="180"/>
+      <c r="BR7" s="180">
         <v>43001</v>
       </c>
-      <c r="BS7" s="174"/>
-      <c r="BT7" s="174">
+      <c r="BS7" s="180"/>
+      <c r="BT7" s="180">
         <v>43022</v>
       </c>
-      <c r="BU7" s="174"/>
-      <c r="BV7" s="174">
+      <c r="BU7" s="180"/>
+      <c r="BV7" s="180">
         <v>43029</v>
       </c>
-      <c r="BW7" s="174"/>
-      <c r="BX7" s="174">
+      <c r="BW7" s="180"/>
+      <c r="BX7" s="180">
         <v>43036</v>
       </c>
-      <c r="BY7" s="174"/>
-      <c r="BZ7" s="174">
+      <c r="BY7" s="180"/>
+      <c r="BZ7" s="180">
         <v>43036</v>
       </c>
-      <c r="CA7" s="174"/>
-      <c r="CB7" s="174">
+      <c r="CA7" s="180"/>
+      <c r="CB7" s="180">
         <v>43050</v>
       </c>
-      <c r="CC7" s="174"/>
-      <c r="CD7" s="174">
+      <c r="CC7" s="180"/>
+      <c r="CD7" s="180">
         <v>43057</v>
       </c>
-      <c r="CE7" s="174"/>
-      <c r="CF7" s="174"/>
-      <c r="CG7" s="174"/>
-      <c r="CH7" s="174"/>
-      <c r="CI7" s="174"/>
-      <c r="CJ7" s="174"/>
-      <c r="CK7" s="174"/>
-      <c r="CL7" s="174"/>
-      <c r="CM7" s="174"/>
-      <c r="CN7" s="180">
+      <c r="CE7" s="180"/>
+      <c r="CF7" s="180"/>
+      <c r="CG7" s="180"/>
+      <c r="CH7" s="180"/>
+      <c r="CI7" s="180"/>
+      <c r="CJ7" s="180"/>
+      <c r="CK7" s="180"/>
+      <c r="CL7" s="180"/>
+      <c r="CM7" s="180"/>
+      <c r="CN7" s="181">
         <f>COUNT(CN9,CL9,CJ9,CH9,CF9,CD9,CB9,BZ9,BX9,BV9,BT9,BR9,BP9,BN9,BL9)</f>
         <v>10</v>
       </c>
-      <c r="CO7" s="180"/>
+      <c r="CO7" s="181"/>
       <c r="CP7" s="100">
         <v>0.5</v>
       </c>
-      <c r="CQ7" s="194"/>
-      <c r="CR7" s="194"/>
-      <c r="CS7" s="190"/>
-      <c r="CT7" s="190"/>
-      <c r="CU7" s="182"/>
+      <c r="CQ7" s="185"/>
+      <c r="CR7" s="185"/>
+      <c r="CS7" s="167"/>
+      <c r="CT7" s="167"/>
+      <c r="CU7" s="190"/>
     </row>
     <row r="8" spans="1:99" ht="15.75" thickBot="1">
-      <c r="A8" s="196"/>
-      <c r="B8" s="198"/>
-      <c r="C8" s="198"/>
-      <c r="D8" s="205" t="s">
+      <c r="A8" s="169"/>
+      <c r="B8" s="171"/>
+      <c r="C8" s="171"/>
+      <c r="D8" s="178" t="s">
         <v>156</v>
       </c>
-      <c r="E8" s="205"/>
-      <c r="F8" s="205"/>
-      <c r="G8" s="205" t="s">
+      <c r="E8" s="178"/>
+      <c r="F8" s="178"/>
+      <c r="G8" s="178" t="s">
         <v>157</v>
       </c>
-      <c r="H8" s="205"/>
-      <c r="I8" s="205"/>
-      <c r="J8" s="167" t="s">
+      <c r="H8" s="178"/>
+      <c r="I8" s="178"/>
+      <c r="J8" s="179" t="s">
         <v>48</v>
       </c>
-      <c r="K8" s="167"/>
-      <c r="L8" s="167" t="s">
+      <c r="K8" s="179"/>
+      <c r="L8" s="179" t="s">
         <v>49</v>
       </c>
-      <c r="M8" s="167"/>
-      <c r="N8" s="167" t="s">
+      <c r="M8" s="179"/>
+      <c r="N8" s="179" t="s">
         <v>50</v>
       </c>
-      <c r="O8" s="167"/>
-      <c r="P8" s="167" t="s">
+      <c r="O8" s="179"/>
+      <c r="P8" s="179" t="s">
         <v>51</v>
       </c>
-      <c r="Q8" s="167"/>
-      <c r="R8" s="167" t="s">
+      <c r="Q8" s="179"/>
+      <c r="R8" s="179" t="s">
         <v>52</v>
       </c>
-      <c r="S8" s="167"/>
-      <c r="T8" s="167" t="s">
+      <c r="S8" s="179"/>
+      <c r="T8" s="179" t="s">
         <v>53</v>
       </c>
-      <c r="U8" s="167"/>
-      <c r="V8" s="167" t="s">
+      <c r="U8" s="179"/>
+      <c r="V8" s="179" t="s">
         <v>54</v>
       </c>
-      <c r="W8" s="167"/>
-      <c r="X8" s="167" t="s">
+      <c r="W8" s="179"/>
+      <c r="X8" s="179" t="s">
         <v>55</v>
       </c>
-      <c r="Y8" s="167"/>
-      <c r="Z8" s="167" t="s">
+      <c r="Y8" s="179"/>
+      <c r="Z8" s="179" t="s">
         <v>56</v>
       </c>
-      <c r="AA8" s="167"/>
-      <c r="AB8" s="167" t="s">
+      <c r="AA8" s="179"/>
+      <c r="AB8" s="179" t="s">
         <v>57</v>
       </c>
-      <c r="AC8" s="167"/>
-      <c r="AD8" s="167" t="s">
+      <c r="AC8" s="179"/>
+      <c r="AD8" s="179" t="s">
         <v>58</v>
       </c>
-      <c r="AE8" s="167"/>
-      <c r="AF8" s="167" t="s">
+      <c r="AE8" s="179"/>
+      <c r="AF8" s="179" t="s">
         <v>59</v>
       </c>
-      <c r="AG8" s="167"/>
-      <c r="AH8" s="167" t="s">
+      <c r="AG8" s="179"/>
+      <c r="AH8" s="179" t="s">
         <v>60</v>
       </c>
-      <c r="AI8" s="167"/>
-      <c r="AJ8" s="167" t="s">
+      <c r="AI8" s="179"/>
+      <c r="AJ8" s="179" t="s">
         <v>61</v>
       </c>
-      <c r="AK8" s="167"/>
-      <c r="AL8" s="167" t="s">
+      <c r="AK8" s="179"/>
+      <c r="AL8" s="179" t="s">
         <v>62</v>
       </c>
-      <c r="AM8" s="167"/>
+      <c r="AM8" s="179"/>
       <c r="AN8" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="AO8" s="167" t="s">
+      <c r="AO8" s="179" t="s">
         <v>64</v>
       </c>
-      <c r="AP8" s="167"/>
-      <c r="AQ8" s="167" t="s">
+      <c r="AP8" s="179"/>
+      <c r="AQ8" s="179" t="s">
         <v>65</v>
       </c>
-      <c r="AR8" s="167"/>
-      <c r="AS8" s="167" t="s">
+      <c r="AR8" s="179"/>
+      <c r="AS8" s="179" t="s">
         <v>66</v>
       </c>
-      <c r="AT8" s="167"/>
+      <c r="AT8" s="179"/>
       <c r="AU8" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="AV8" s="167" t="s">
+      <c r="AV8" s="179" t="s">
         <v>68</v>
       </c>
-      <c r="AW8" s="167"/>
-      <c r="AX8" s="167" t="s">
+      <c r="AW8" s="179"/>
+      <c r="AX8" s="179" t="s">
         <v>69</v>
       </c>
-      <c r="AY8" s="167"/>
-      <c r="AZ8" s="167" t="s">
+      <c r="AY8" s="179"/>
+      <c r="AZ8" s="179" t="s">
         <v>70</v>
       </c>
-      <c r="BA8" s="167"/>
+      <c r="BA8" s="179"/>
       <c r="BB8" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="BC8" s="184"/>
-      <c r="BD8" s="185"/>
-      <c r="BE8" s="177" t="s">
+      <c r="BC8" s="192"/>
+      <c r="BD8" s="193"/>
+      <c r="BE8" s="203" t="s">
         <v>44</v>
       </c>
-      <c r="BF8" s="176"/>
-      <c r="BG8" s="176" t="s">
+      <c r="BF8" s="200"/>
+      <c r="BG8" s="200" t="s">
         <v>45</v>
       </c>
-      <c r="BH8" s="176"/>
-      <c r="BI8" s="176" t="s">
+      <c r="BH8" s="200"/>
+      <c r="BI8" s="200" t="s">
         <v>46</v>
       </c>
-      <c r="BJ8" s="176"/>
+      <c r="BJ8" s="200"/>
       <c r="BK8" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="BL8" s="170" t="s">
+      <c r="BL8" s="201" t="s">
         <v>72</v>
       </c>
-      <c r="BM8" s="171"/>
-      <c r="BN8" s="170" t="s">
+      <c r="BM8" s="202"/>
+      <c r="BN8" s="201" t="s">
         <v>73</v>
       </c>
-      <c r="BO8" s="171"/>
-      <c r="BP8" s="170" t="s">
+      <c r="BO8" s="202"/>
+      <c r="BP8" s="201" t="s">
         <v>74</v>
       </c>
-      <c r="BQ8" s="171"/>
-      <c r="BR8" s="170" t="s">
+      <c r="BQ8" s="202"/>
+      <c r="BR8" s="201" t="s">
         <v>75</v>
       </c>
-      <c r="BS8" s="171"/>
-      <c r="BT8" s="170" t="s">
+      <c r="BS8" s="202"/>
+      <c r="BT8" s="201" t="s">
         <v>76</v>
       </c>
-      <c r="BU8" s="171"/>
-      <c r="BV8" s="168" t="s">
+      <c r="BU8" s="202"/>
+      <c r="BV8" s="186" t="s">
         <v>77</v>
       </c>
-      <c r="BW8" s="169"/>
-      <c r="BX8" s="168" t="s">
+      <c r="BW8" s="187"/>
+      <c r="BX8" s="186" t="s">
         <v>78</v>
       </c>
-      <c r="BY8" s="169"/>
-      <c r="BZ8" s="168" t="s">
+      <c r="BY8" s="187"/>
+      <c r="BZ8" s="186" t="s">
         <v>79</v>
       </c>
-      <c r="CA8" s="169"/>
-      <c r="CB8" s="168" t="s">
+      <c r="CA8" s="187"/>
+      <c r="CB8" s="186" t="s">
         <v>80</v>
       </c>
-      <c r="CC8" s="169"/>
-      <c r="CD8" s="168" t="s">
+      <c r="CC8" s="187"/>
+      <c r="CD8" s="186" t="s">
         <v>81</v>
       </c>
-      <c r="CE8" s="169"/>
-      <c r="CF8" s="168" t="s">
+      <c r="CE8" s="187"/>
+      <c r="CF8" s="186" t="s">
         <v>82</v>
       </c>
-      <c r="CG8" s="169"/>
-      <c r="CH8" s="168" t="s">
+      <c r="CG8" s="187"/>
+      <c r="CH8" s="186" t="s">
         <v>83</v>
       </c>
-      <c r="CI8" s="169"/>
-      <c r="CJ8" s="168" t="s">
+      <c r="CI8" s="187"/>
+      <c r="CJ8" s="186" t="s">
         <v>84</v>
       </c>
-      <c r="CK8" s="169"/>
-      <c r="CL8" s="168" t="s">
+      <c r="CK8" s="187"/>
+      <c r="CL8" s="186" t="s">
         <v>85</v>
       </c>
-      <c r="CM8" s="169"/>
-      <c r="CN8" s="168" t="s">
+      <c r="CM8" s="187"/>
+      <c r="CN8" s="186" t="s">
         <v>86</v>
       </c>
-      <c r="CO8" s="169"/>
+      <c r="CO8" s="187"/>
       <c r="CP8" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="CQ8" s="194"/>
-      <c r="CR8" s="194"/>
-      <c r="CS8" s="190"/>
-      <c r="CT8" s="190"/>
-      <c r="CU8" s="182"/>
+      <c r="CQ8" s="185"/>
+      <c r="CR8" s="185"/>
+      <c r="CS8" s="167"/>
+      <c r="CT8" s="167"/>
+      <c r="CU8" s="190"/>
     </row>
     <row r="9" spans="1:99" ht="15.75" thickBot="1">
-      <c r="A9" s="197"/>
-      <c r="B9" s="198"/>
-      <c r="C9" s="198"/>
+      <c r="A9" s="170"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="171"/>
       <c r="D9" s="27">
         <v>100</v>
       </c>
@@ -8349,9 +8349,9 @@
       <c r="CR9" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="CS9" s="190"/>
-      <c r="CT9" s="190"/>
-      <c r="CU9" s="183"/>
+      <c r="CS9" s="167"/>
+      <c r="CT9" s="167"/>
+      <c r="CU9" s="191"/>
     </row>
     <row r="10" spans="1:99">
       <c r="A10" s="42">
@@ -24798,6 +24798,88 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="98">
+    <mergeCell ref="AD8:AE8"/>
+    <mergeCell ref="AJ8:AK8"/>
+    <mergeCell ref="AV8:AW8"/>
+    <mergeCell ref="AX8:AY8"/>
+    <mergeCell ref="A2:CU3"/>
+    <mergeCell ref="CB8:CC8"/>
+    <mergeCell ref="CD8:CE8"/>
+    <mergeCell ref="CF8:CG8"/>
+    <mergeCell ref="CH8:CI8"/>
+    <mergeCell ref="CJ8:CK8"/>
+    <mergeCell ref="CL8:CM8"/>
+    <mergeCell ref="BP8:BQ8"/>
+    <mergeCell ref="BR8:BS8"/>
+    <mergeCell ref="BT8:BU8"/>
+    <mergeCell ref="BV8:BW8"/>
+    <mergeCell ref="BX8:BY8"/>
+    <mergeCell ref="BZ8:CA8"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="X8:Y8"/>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="AB8:AC8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="J6:AN6"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="AF8:AG8"/>
+    <mergeCell ref="AH8:AI8"/>
+    <mergeCell ref="BI8:BJ8"/>
+    <mergeCell ref="BL8:BM8"/>
+    <mergeCell ref="BN8:BO8"/>
+    <mergeCell ref="AL8:AM8"/>
+    <mergeCell ref="AO8:AP8"/>
+    <mergeCell ref="AQ8:AR8"/>
+    <mergeCell ref="AS8:AT8"/>
+    <mergeCell ref="BE8:BF8"/>
+    <mergeCell ref="AZ8:BA8"/>
+    <mergeCell ref="BG8:BH8"/>
+    <mergeCell ref="BI7:BJ7"/>
+    <mergeCell ref="AH7:AI7"/>
+    <mergeCell ref="AJ7:AK7"/>
+    <mergeCell ref="AL7:AM7"/>
+    <mergeCell ref="AO7:AP7"/>
+    <mergeCell ref="AQ7:AR7"/>
+    <mergeCell ref="AS7:AT7"/>
+    <mergeCell ref="AO6:AU6"/>
+    <mergeCell ref="AV6:BB6"/>
+    <mergeCell ref="CU6:CU9"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="BC6:BD8"/>
+    <mergeCell ref="BE6:BK6"/>
+    <mergeCell ref="BL6:CP6"/>
+    <mergeCell ref="AD7:AE7"/>
+    <mergeCell ref="AF7:AG7"/>
+    <mergeCell ref="CT6:CT9"/>
+    <mergeCell ref="BE7:BF7"/>
+    <mergeCell ref="CS5:CU5"/>
+    <mergeCell ref="BL7:BM7"/>
+    <mergeCell ref="BN7:BO7"/>
+    <mergeCell ref="BP7:BQ7"/>
+    <mergeCell ref="BR7:BS7"/>
+    <mergeCell ref="CL7:CM7"/>
+    <mergeCell ref="CN7:CO7"/>
+    <mergeCell ref="BT7:BU7"/>
+    <mergeCell ref="BV7:BW7"/>
+    <mergeCell ref="BX7:BY7"/>
+    <mergeCell ref="BZ7:CA7"/>
+    <mergeCell ref="CB7:CC7"/>
+    <mergeCell ref="CJ7:CK7"/>
+    <mergeCell ref="CD7:CE7"/>
+    <mergeCell ref="CQ6:CR8"/>
+    <mergeCell ref="CN8:CO8"/>
     <mergeCell ref="CS6:CS9"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="B5:B9"/>
@@ -24814,88 +24896,6 @@
     <mergeCell ref="BG7:BH7"/>
     <mergeCell ref="CF7:CG7"/>
     <mergeCell ref="CH7:CI7"/>
-    <mergeCell ref="CS5:CU5"/>
-    <mergeCell ref="BL7:BM7"/>
-    <mergeCell ref="BN7:BO7"/>
-    <mergeCell ref="BP7:BQ7"/>
-    <mergeCell ref="BR7:BS7"/>
-    <mergeCell ref="CL7:CM7"/>
-    <mergeCell ref="CN7:CO7"/>
-    <mergeCell ref="BT7:BU7"/>
-    <mergeCell ref="BV7:BW7"/>
-    <mergeCell ref="BX7:BY7"/>
-    <mergeCell ref="BZ7:CA7"/>
-    <mergeCell ref="CB7:CC7"/>
-    <mergeCell ref="CJ7:CK7"/>
-    <mergeCell ref="CD7:CE7"/>
-    <mergeCell ref="CQ6:CR8"/>
-    <mergeCell ref="CN8:CO8"/>
-    <mergeCell ref="AO6:AU6"/>
-    <mergeCell ref="AV6:BB6"/>
-    <mergeCell ref="CU6:CU9"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="BC6:BD8"/>
-    <mergeCell ref="BE6:BK6"/>
-    <mergeCell ref="BL6:CP6"/>
-    <mergeCell ref="AD7:AE7"/>
-    <mergeCell ref="AF7:AG7"/>
-    <mergeCell ref="CT6:CT9"/>
-    <mergeCell ref="BE7:BF7"/>
-    <mergeCell ref="BI7:BJ7"/>
-    <mergeCell ref="AH7:AI7"/>
-    <mergeCell ref="AJ7:AK7"/>
-    <mergeCell ref="AL7:AM7"/>
-    <mergeCell ref="AO7:AP7"/>
-    <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="AS7:AT7"/>
-    <mergeCell ref="AH8:AI8"/>
-    <mergeCell ref="BI8:BJ8"/>
-    <mergeCell ref="BL8:BM8"/>
-    <mergeCell ref="BN8:BO8"/>
-    <mergeCell ref="AL8:AM8"/>
-    <mergeCell ref="AO8:AP8"/>
-    <mergeCell ref="AQ8:AR8"/>
-    <mergeCell ref="AS8:AT8"/>
-    <mergeCell ref="BE8:BF8"/>
-    <mergeCell ref="AZ8:BA8"/>
-    <mergeCell ref="BG8:BH8"/>
-    <mergeCell ref="BZ8:CA8"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="X8:Y8"/>
-    <mergeCell ref="Z8:AA8"/>
-    <mergeCell ref="AB8:AC8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="X7:Y7"/>
-    <mergeCell ref="Z7:AA7"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="J6:AN6"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="AF8:AG8"/>
-    <mergeCell ref="AD8:AE8"/>
-    <mergeCell ref="AJ8:AK8"/>
-    <mergeCell ref="AV8:AW8"/>
-    <mergeCell ref="AX8:AY8"/>
-    <mergeCell ref="A2:CU3"/>
-    <mergeCell ref="CB8:CC8"/>
-    <mergeCell ref="CD8:CE8"/>
-    <mergeCell ref="CF8:CG8"/>
-    <mergeCell ref="CH8:CI8"/>
-    <mergeCell ref="CJ8:CK8"/>
-    <mergeCell ref="CL8:CM8"/>
-    <mergeCell ref="BP8:BQ8"/>
-    <mergeCell ref="BR8:BS8"/>
-    <mergeCell ref="BT8:BU8"/>
-    <mergeCell ref="BV8:BW8"/>
-    <mergeCell ref="BX8:BY8"/>
   </mergeCells>
   <conditionalFormatting sqref="CU10:CU70">
     <cfRule type="cellIs" dxfId="46" priority="1" operator="equal">
@@ -24920,7 +24920,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:P68"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
       <selection sqref="A1:P40"/>
     </sheetView>
   </sheetViews>
@@ -29073,7 +29073,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="72" orientation="landscape" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
+  <pageSetup paperSize="256" scale="85" orientation="landscape" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -29111,106 +29111,106 @@
       <c r="F2" s="60"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="253"/>
-      <c r="B3" s="253"/>
-      <c r="C3" s="253"/>
-      <c r="D3" s="253"/>
-      <c r="E3" s="253"/>
-      <c r="F3" s="253"/>
+      <c r="A3" s="222"/>
+      <c r="B3" s="222"/>
+      <c r="C3" s="222"/>
+      <c r="D3" s="222"/>
+      <c r="E3" s="222"/>
+      <c r="F3" s="222"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="256" t="s">
+      <c r="A4" s="223" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="256"/>
-      <c r="C4" s="256"/>
-      <c r="D4" s="256"/>
-      <c r="E4" s="256"/>
-      <c r="F4" s="256"/>
+      <c r="B4" s="223"/>
+      <c r="C4" s="223"/>
+      <c r="D4" s="223"/>
+      <c r="E4" s="223"/>
+      <c r="F4" s="223"/>
     </row>
     <row r="5" spans="1:6" ht="18">
-      <c r="A5" s="257" t="s">
+      <c r="A5" s="224" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="257"/>
-      <c r="C5" s="257"/>
-      <c r="D5" s="257"/>
-      <c r="E5" s="257"/>
-      <c r="F5" s="257"/>
+      <c r="B5" s="224"/>
+      <c r="C5" s="224"/>
+      <c r="D5" s="224"/>
+      <c r="E5" s="224"/>
+      <c r="F5" s="224"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="256" t="s">
+      <c r="A6" s="223" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="256"/>
-      <c r="C6" s="256"/>
-      <c r="D6" s="256"/>
-      <c r="E6" s="256"/>
-      <c r="F6" s="256"/>
+      <c r="B6" s="223"/>
+      <c r="C6" s="223"/>
+      <c r="D6" s="223"/>
+      <c r="E6" s="223"/>
+      <c r="F6" s="223"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="258" t="s">
+      <c r="A7" s="225" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="258"/>
-      <c r="C7" s="258"/>
-      <c r="D7" s="258"/>
-      <c r="E7" s="258"/>
-      <c r="F7" s="258"/>
+      <c r="B7" s="225"/>
+      <c r="C7" s="225"/>
+      <c r="D7" s="225"/>
+      <c r="E7" s="225"/>
+      <c r="F7" s="225"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="259"/>
-      <c r="B8" s="259"/>
-      <c r="C8" s="259"/>
-      <c r="D8" s="259"/>
-      <c r="E8" s="259"/>
-      <c r="F8" s="259"/>
+      <c r="A8" s="226"/>
+      <c r="B8" s="226"/>
+      <c r="C8" s="226"/>
+      <c r="D8" s="226"/>
+      <c r="E8" s="226"/>
+      <c r="F8" s="226"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="253"/>
-      <c r="B9" s="253"/>
-      <c r="C9" s="253"/>
-      <c r="D9" s="253"/>
-      <c r="E9" s="253"/>
-      <c r="F9" s="253"/>
+      <c r="A9" s="222"/>
+      <c r="B9" s="222"/>
+      <c r="C9" s="222"/>
+      <c r="D9" s="222"/>
+      <c r="E9" s="222"/>
+      <c r="F9" s="222"/>
     </row>
     <row r="10" spans="1:6" ht="18">
-      <c r="A10" s="260"/>
-      <c r="B10" s="260"/>
-      <c r="C10" s="260"/>
-      <c r="D10" s="260"/>
-      <c r="E10" s="260"/>
-      <c r="F10" s="260"/>
+      <c r="A10" s="227"/>
+      <c r="B10" s="227"/>
+      <c r="C10" s="227"/>
+      <c r="D10" s="227"/>
+      <c r="E10" s="227"/>
+      <c r="F10" s="227"/>
     </row>
     <row r="11" spans="1:6" ht="22.5">
-      <c r="A11" s="261" t="s">
+      <c r="A11" s="228" t="s">
         <v>110</v>
       </c>
-      <c r="B11" s="261"/>
-      <c r="C11" s="261"/>
-      <c r="D11" s="261"/>
-      <c r="E11" s="261"/>
-      <c r="F11" s="261"/>
+      <c r="B11" s="228"/>
+      <c r="C11" s="228"/>
+      <c r="D11" s="228"/>
+      <c r="E11" s="228"/>
+      <c r="F11" s="228"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="259"/>
-      <c r="B12" s="259"/>
-      <c r="C12" s="259"/>
-      <c r="D12" s="259"/>
-      <c r="E12" s="259"/>
-      <c r="F12" s="259"/>
+      <c r="A12" s="226"/>
+      <c r="B12" s="226"/>
+      <c r="C12" s="226"/>
+      <c r="D12" s="226"/>
+      <c r="E12" s="226"/>
+      <c r="F12" s="226"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="60"/>
       <c r="B13" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="262" t="str">
+      <c r="C13" s="229" t="str">
         <f>REGISTRATION!C7</f>
         <v>DCIT 65</v>
       </c>
-      <c r="D13" s="262"/>
-      <c r="E13" s="262"/>
+      <c r="D13" s="229"/>
+      <c r="E13" s="229"/>
       <c r="F13" s="62"/>
     </row>
     <row r="14" spans="1:6">
@@ -29218,12 +29218,12 @@
       <c r="B14" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="255" t="str">
+      <c r="C14" s="221" t="str">
         <f>REGISTRATION!C6</f>
         <v>Web Development</v>
       </c>
-      <c r="D14" s="255"/>
-      <c r="E14" s="255"/>
+      <c r="D14" s="221"/>
+      <c r="E14" s="221"/>
       <c r="F14" s="62"/>
     </row>
     <row r="15" spans="1:6">
@@ -29231,12 +29231,12 @@
       <c r="B15" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="241" t="str">
+      <c r="C15" s="232" t="str">
         <f>REGISTRATION!A4</f>
         <v>THIRD YEAR</v>
       </c>
-      <c r="D15" s="241"/>
-      <c r="E15" s="241"/>
+      <c r="D15" s="232"/>
+      <c r="E15" s="232"/>
       <c r="F15" s="63"/>
     </row>
     <row r="16" spans="1:6">
@@ -29244,12 +29244,12 @@
       <c r="B16" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="241" t="str">
+      <c r="C16" s="232" t="str">
         <f>UPPER(CONCATENATE(REGISTRATION!C8," ",REGISTRATION!D8))</f>
         <v>CS 3A</v>
       </c>
-      <c r="D16" s="241"/>
-      <c r="E16" s="241"/>
+      <c r="D16" s="232"/>
+      <c r="E16" s="232"/>
       <c r="F16" s="63"/>
     </row>
     <row r="17" spans="1:6">
@@ -29257,12 +29257,12 @@
       <c r="B17" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="C17" s="241" t="str">
+      <c r="C17" s="232" t="str">
         <f>UPPER(CONCATENATE(REGISTRATION!P13," ","SEMESTER"," ","A.Y."," ",REGISTRATION!P12))</f>
         <v>FIRST SEMESTER A.Y. 2017-2018</v>
       </c>
-      <c r="D17" s="241"/>
-      <c r="E17" s="241"/>
+      <c r="D17" s="232"/>
+      <c r="E17" s="232"/>
       <c r="F17" s="63"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1">
@@ -29274,42 +29274,42 @@
       <c r="F18" s="60"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="242" t="s">
+      <c r="A19" s="233" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="245" t="s">
+      <c r="B19" s="236" t="s">
         <v>92</v>
       </c>
-      <c r="C19" s="242" t="s">
+      <c r="C19" s="233" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="242" t="s">
+      <c r="D19" s="233" t="s">
         <v>115</v>
       </c>
-      <c r="E19" s="247" t="s">
+      <c r="E19" s="238" t="s">
         <v>116</v>
       </c>
-      <c r="F19" s="242" t="s">
+      <c r="F19" s="233" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="243"/>
-      <c r="B20" s="246"/>
-      <c r="C20" s="243"/>
-      <c r="D20" s="243"/>
-      <c r="E20" s="248"/>
-      <c r="F20" s="250"/>
+      <c r="A20" s="234"/>
+      <c r="B20" s="237"/>
+      <c r="C20" s="234"/>
+      <c r="D20" s="234"/>
+      <c r="E20" s="239"/>
+      <c r="F20" s="241"/>
     </row>
     <row r="21" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A21" s="244"/>
+      <c r="A21" s="235"/>
       <c r="B21" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="C21" s="244"/>
-      <c r="D21" s="244"/>
-      <c r="E21" s="249"/>
-      <c r="F21" s="251"/>
+      <c r="C21" s="235"/>
+      <c r="D21" s="235"/>
+      <c r="E21" s="240"/>
+      <c r="F21" s="242"/>
     </row>
     <row r="22" spans="1:6" ht="18">
       <c r="A22" s="65">
@@ -30137,14 +30137,14 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="19.5" thickBot="1">
-      <c r="A55" s="225" t="s">
+      <c r="A55" s="249" t="s">
         <v>118</v>
       </c>
-      <c r="B55" s="226"/>
-      <c r="C55" s="226"/>
-      <c r="D55" s="226"/>
-      <c r="E55" s="226"/>
-      <c r="F55" s="227"/>
+      <c r="B55" s="250"/>
+      <c r="C55" s="250"/>
+      <c r="D55" s="250"/>
+      <c r="E55" s="250"/>
+      <c r="F55" s="251"/>
     </row>
     <row r="56" spans="1:6" ht="15.75">
       <c r="A56" s="62"/>
@@ -30177,11 +30177,11 @@
       </c>
       <c r="C59" s="60"/>
       <c r="D59" s="60"/>
-      <c r="E59" s="252">
+      <c r="E59" s="243">
         <f ca="1">NOW()</f>
-        <v>43081.87773078704</v>
-      </c>
-      <c r="F59" s="252"/>
+        <v>43082.761145370372</v>
+      </c>
+      <c r="F59" s="243"/>
     </row>
     <row r="60" spans="1:6" ht="15.75">
       <c r="A60" s="60"/>
@@ -30191,10 +30191,10 @@
       </c>
       <c r="C60" s="73"/>
       <c r="D60" s="73"/>
-      <c r="E60" s="253" t="s">
+      <c r="E60" s="222" t="s">
         <v>120</v>
       </c>
-      <c r="F60" s="253"/>
+      <c r="F60" s="222"/>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="60"/>
@@ -30211,8 +30211,8 @@
       <c r="B62" s="74"/>
       <c r="C62" s="74"/>
       <c r="D62" s="74"/>
-      <c r="E62" s="253"/>
-      <c r="F62" s="253"/>
+      <c r="E62" s="222"/>
+      <c r="F62" s="222"/>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="60"/>
@@ -30327,14 +30327,14 @@
       <c r="F76" s="60"/>
     </row>
     <row r="77" spans="1:6" ht="15.75">
-      <c r="A77" s="254" t="s">
+      <c r="A77" s="244" t="s">
         <v>135</v>
       </c>
-      <c r="B77" s="254"/>
-      <c r="C77" s="254"/>
-      <c r="D77" s="254"/>
-      <c r="E77" s="254"/>
-      <c r="F77" s="254"/>
+      <c r="B77" s="244"/>
+      <c r="C77" s="244"/>
+      <c r="D77" s="244"/>
+      <c r="E77" s="244"/>
+      <c r="F77" s="244"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" thickBot="1">
       <c r="A78" s="60"/>
@@ -30349,124 +30349,124 @@
       <c r="B79" s="78" t="s">
         <v>136</v>
       </c>
-      <c r="C79" s="238" t="s">
+      <c r="C79" s="262" t="s">
         <v>137</v>
       </c>
-      <c r="D79" s="239"/>
-      <c r="E79" s="240" t="s">
+      <c r="D79" s="231"/>
+      <c r="E79" s="230" t="s">
         <v>138</v>
       </c>
-      <c r="F79" s="239"/>
+      <c r="F79" s="231"/>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="60"/>
       <c r="B80" s="80" t="s">
         <v>122</v>
       </c>
-      <c r="C80" s="234">
+      <c r="C80" s="258">
         <f>COUNTIF($D$22:$D$54,"=1.0")+COUNTIF($D$22:$D$54,"=1.25")+(COUNTIF($D$22:$D$54,"=1.50")+COUNTIF($D$22:$D$54,"=1.75"))</f>
         <v>8</v>
       </c>
-      <c r="D80" s="235"/>
-      <c r="E80" s="236">
+      <c r="D80" s="259"/>
+      <c r="E80" s="260">
         <f>(C80/$C$86)*100</f>
         <v>24.242424242424242</v>
       </c>
-      <c r="F80" s="237"/>
+      <c r="F80" s="261"/>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="60"/>
       <c r="B81" s="81" t="s">
         <v>123</v>
       </c>
-      <c r="C81" s="228">
+      <c r="C81" s="252">
         <f>COUNTIF($D$22:$D$54,"=2.0")+COUNTIF($D$22:$D$54,"=2.25")+(COUNTIF($D$22:$D$54,"=2.50")+COUNTIF($D$22:$D$54,"=2.75"))</f>
         <v>20</v>
       </c>
-      <c r="D81" s="229"/>
-      <c r="E81" s="230">
+      <c r="D81" s="253"/>
+      <c r="E81" s="254">
         <f>(C81/$C$86)*100</f>
         <v>60.606060606060609</v>
       </c>
-      <c r="F81" s="231"/>
+      <c r="F81" s="255"/>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="60"/>
       <c r="B82" s="81" t="s">
         <v>124</v>
       </c>
-      <c r="C82" s="228">
+      <c r="C82" s="252">
         <f>COUNTIF($D$22:$D$54,"=3.0")</f>
         <v>4</v>
       </c>
-      <c r="D82" s="229"/>
-      <c r="E82" s="230">
+      <c r="D82" s="253"/>
+      <c r="E82" s="254">
         <f t="shared" ref="E82:E85" si="1">(C82/$C$86)*100</f>
         <v>12.121212121212121</v>
       </c>
-      <c r="F82" s="231"/>
+      <c r="F82" s="255"/>
     </row>
     <row r="83" spans="1:6" ht="15.75" customHeight="1">
       <c r="A83" s="60"/>
       <c r="B83" s="81" t="s">
         <v>125</v>
       </c>
-      <c r="C83" s="228">
+      <c r="C83" s="252">
         <f>COUNTIF($D$22:$D$54,"=5.0")</f>
         <v>1</v>
       </c>
-      <c r="D83" s="229"/>
-      <c r="E83" s="230">
+      <c r="D83" s="253"/>
+      <c r="E83" s="254">
         <f t="shared" si="1"/>
         <v>3.0303030303030303</v>
       </c>
-      <c r="F83" s="231"/>
+      <c r="F83" s="255"/>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="60"/>
       <c r="B84" s="81" t="s">
         <v>126</v>
       </c>
-      <c r="C84" s="232">
-        <v>0</v>
-      </c>
-      <c r="D84" s="233"/>
-      <c r="E84" s="230">
+      <c r="C84" s="256">
+        <v>0</v>
+      </c>
+      <c r="D84" s="257"/>
+      <c r="E84" s="254">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F84" s="231"/>
+      <c r="F84" s="255"/>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="60"/>
       <c r="B85" s="81" t="s">
         <v>127</v>
       </c>
-      <c r="C85" s="232">
-        <v>0</v>
-      </c>
-      <c r="D85" s="233"/>
-      <c r="E85" s="230">
+      <c r="C85" s="256">
+        <v>0</v>
+      </c>
+      <c r="D85" s="257"/>
+      <c r="E85" s="254">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F85" s="231"/>
+      <c r="F85" s="255"/>
     </row>
     <row r="86" spans="1:6" ht="16.5" thickBot="1">
       <c r="A86" s="60"/>
       <c r="B86" s="82" t="s">
         <v>128</v>
       </c>
-      <c r="C86" s="221">
+      <c r="C86" s="245">
         <f>SUM(C80:D85)</f>
         <v>33</v>
       </c>
-      <c r="D86" s="222"/>
-      <c r="E86" s="223">
+      <c r="D86" s="246"/>
+      <c r="E86" s="247">
         <f>SUM(E80:F85)</f>
         <v>100</v>
       </c>
-      <c r="F86" s="224"/>
+      <c r="F86" s="248"/>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="60"/>
@@ -30634,32 +30634,6 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="E79:F79"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="A77:F77"/>
     <mergeCell ref="C86:D86"/>
     <mergeCell ref="E86:F86"/>
     <mergeCell ref="A55:F55"/>
@@ -30676,6 +30650,32 @@
     <mergeCell ref="C82:D82"/>
     <mergeCell ref="E82:F82"/>
     <mergeCell ref="C79:D79"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="A77:F77"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="C13:E13"/>
   </mergeCells>
   <conditionalFormatting sqref="F22:F54">
     <cfRule type="cellIs" dxfId="44" priority="1" operator="equal">
@@ -30683,7 +30683,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="58" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="58" orientation="portrait" horizontalDpi="4294967294" verticalDpi="360" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="72" max="16383" man="1"/>
   </rowBreaks>

</xml_diff>